<commit_message>
fix real value in plot, update 07.31 data
</commit_message>
<xml_diff>
--- a/COVID-19/HCM/SEIRD_data_12_7_2021.xlsx
+++ b/COVID-19/HCM/SEIRD_data_12_7_2021.xlsx
@@ -247,7 +247,7 @@
   <dimension ref="A1:X83"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A63" activeCellId="0" sqref="A63:X64"/>
+      <selection pane="topLeft" activeCell="B65" activeCellId="0" sqref="A65:X66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4998,10 +4998,154 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3"/>
+      <c r="A65" s="3" t="n">
+        <v>44041</v>
+      </c>
+      <c r="B65" s="5" t="n">
+        <f aca="false">SUM(C65:X65)</f>
+        <v>596</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D65" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E65" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="F65" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="G65" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="H65" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="I65" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="J65" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="K65" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L65" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="M65" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="N65" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="O65" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="P65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R65" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="S65" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="T65" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="U65" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="V65" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="W65" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="X65" s="1" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3"/>
+      <c r="A66" s="3" t="n">
+        <v>44042</v>
+      </c>
+      <c r="B66" s="5" t="n">
+        <f aca="false">SUM(C66:X66)</f>
+        <v>331</v>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D66" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E66" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="F66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="H66" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I66" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="J66" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M66" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="N66" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="O66" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="R66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S66" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="T66" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="U66" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="V66" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="W66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X66" s="1" t="n">
+        <v>65</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
@@ -5073,7 +5217,7 @@
   <dimension ref="A1:Z83"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="A63:X64"/>
+      <selection pane="topLeft" activeCell="B65" activeCellId="0" sqref="A65:X66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9870,10 +10014,154 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3"/>
+      <c r="A65" s="3" t="n">
+        <v>44406</v>
+      </c>
+      <c r="B65" s="1" t="n">
+        <f aca="false">SUM(C65:X65)</f>
+        <v>3968</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="D65" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="E65" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F65" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="G65" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="H65" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="I65" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="J65" s="1" t="n">
+        <v>456</v>
+      </c>
+      <c r="K65" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="L65" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="M65" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="N65" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="O65" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="P65" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="R65" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="S65" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="T65" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="U65" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="V65" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="W65" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="X65" s="1" t="n">
+        <v>283</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3"/>
+      <c r="A66" s="3" t="n">
+        <v>44407</v>
+      </c>
+      <c r="B66" s="1" t="n">
+        <f aca="false">SUM(C66:X66)</f>
+        <v>3761</v>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="D66" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="E66" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="F66" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="G66" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="H66" s="1" t="n">
+        <v>524</v>
+      </c>
+      <c r="I66" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="J66" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="K66" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="L66" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="M66" s="1" t="n">
+        <v>455</v>
+      </c>
+      <c r="N66" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="O66" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="P66" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q66" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="R66" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="S66" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="T66" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="U66" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="V66" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="W66" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="X66" s="1" t="n">
+        <v>364</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
@@ -9942,13 +10230,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X64"/>
+  <dimension ref="A1:X66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="A63:X64"/>
+      <selection pane="topLeft" activeCell="B65" activeCellId="0" sqref="A65:X66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="6" width="11.57"/>
   </cols>
@@ -14692,6 +14980,156 @@
       </c>
       <c r="X64" s="6" t="n">
         <v>873</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="7" t="n">
+        <v>44406</v>
+      </c>
+      <c r="B65" s="6" t="n">
+        <f aca="false">SUM(C65:X65)</f>
+        <v>3851</v>
+      </c>
+      <c r="C65" s="6" t="n">
+        <v>189</v>
+      </c>
+      <c r="D65" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="6" t="n">
+        <v>203</v>
+      </c>
+      <c r="G65" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" s="6" t="n">
+        <v>266</v>
+      </c>
+      <c r="K65" s="6" t="n">
+        <v>261</v>
+      </c>
+      <c r="L65" s="6" t="n">
+        <v>353</v>
+      </c>
+      <c r="M65" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N65" s="6" t="n">
+        <v>794</v>
+      </c>
+      <c r="O65" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P65" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R65" s="6" t="n">
+        <v>748</v>
+      </c>
+      <c r="S65" s="6" t="n">
+        <v>88</v>
+      </c>
+      <c r="T65" s="6" t="n">
+        <v>173</v>
+      </c>
+      <c r="U65" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V65" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="W65" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="X65" s="6" t="n">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="7" t="n">
+        <v>44407</v>
+      </c>
+      <c r="B66" s="6" t="n">
+        <f aca="false">SUM(C66:X66)</f>
+        <v>3128</v>
+      </c>
+      <c r="C66" s="6" t="n">
+        <v>154</v>
+      </c>
+      <c r="D66" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="6" t="n">
+        <v>165</v>
+      </c>
+      <c r="G66" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="6" t="n">
+        <v>216</v>
+      </c>
+      <c r="K66" s="6" t="n">
+        <v>212</v>
+      </c>
+      <c r="L66" s="6" t="n">
+        <v>287</v>
+      </c>
+      <c r="M66" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N66" s="6" t="n">
+        <v>646</v>
+      </c>
+      <c r="O66" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R66" s="6" t="n">
+        <v>608</v>
+      </c>
+      <c r="S66" s="6" t="n">
+        <v>71</v>
+      </c>
+      <c r="T66" s="6" t="n">
+        <v>140</v>
+      </c>
+      <c r="U66" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V66" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W66" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X66" s="6" t="n">
+        <v>628</v>
       </c>
     </row>
   </sheetData>
@@ -14712,11 +15150,11 @@
   </sheetPr>
   <dimension ref="A1:X82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="A63:X64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B65" activeCellId="0" sqref="A65:X66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="1" width="11.57"/>
   </cols>
@@ -19501,10 +19939,154 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3"/>
+      <c r="A65" s="3" t="n">
+        <v>44406</v>
+      </c>
+      <c r="B65" s="1" t="n">
+        <f aca="false">SUM(C65:X65)</f>
+        <v>115</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K65" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="L65" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N65" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="O65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R65" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="S65" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="T65" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="U65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X65" s="1" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3"/>
+      <c r="A66" s="3" t="n">
+        <v>44407</v>
+      </c>
+      <c r="B66" s="1" t="n">
+        <f aca="false">SUM(C66:X66)</f>
+        <v>129</v>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K66" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L66" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="M66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="O66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R66" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="S66" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="T66" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="U66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X66" s="1" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
@@ -19573,10 +20155,10 @@
   <dimension ref="A1:X86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A63" activeCellId="0" sqref="A63:X64"/>
+      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65:X66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
   </cols>
@@ -25766,11 +26348,199 @@
         <v>1161342</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3"/>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="n">
+        <v>44406</v>
+      </c>
+      <c r="B65" s="8" t="n">
+        <f aca="false">8926959 -SUM(Infectious!B65,Deaths!B65)</f>
+        <v>8922876</v>
+      </c>
+      <c r="C65" s="9" t="n">
+        <f aca="false">139485-SUM(Infectious!C65,Deaths!C65)</f>
+        <v>139427</v>
+      </c>
+      <c r="D65" s="8" t="n">
+        <f aca="false">189258--SUM(Infectious!D65,Deaths!D65)</f>
+        <v>189348</v>
+      </c>
+      <c r="E65" s="8" t="n">
+        <f aca="false">173970-SUM(Infectious!E65,Deaths!E65)</f>
+        <v>173967</v>
+      </c>
+      <c r="F65" s="8" t="n">
+        <f aca="false">157920-SUM(Infectious!F65,Deaths!F65)</f>
+        <v>157759</v>
+      </c>
+      <c r="G65" s="8" t="n">
+        <f aca="false">232077-SUM(Infectious!G65,Deaths!G65)</f>
+        <v>231920</v>
+      </c>
+      <c r="H65" s="8" t="n">
+        <f aca="false">356380-SUM(Infectious!H65,Deaths!H65)</f>
+        <v>356139</v>
+      </c>
+      <c r="I65" s="8" t="n">
+        <f aca="false">422151-SUM(Infectious!I65,Deaths!I65)</f>
+        <v>421941</v>
+      </c>
+      <c r="J65" s="8" t="n">
+        <f aca="false">233223-SUM(Infectious!J65,Deaths!J65)</f>
+        <v>232759</v>
+      </c>
+      <c r="K65" s="8" t="n">
+        <f aca="false">208680-SUM(Infectious!K65,Deaths!K65)</f>
+        <v>208484</v>
+      </c>
+      <c r="L65" s="8" t="n">
+        <f aca="false">618365-SUM(Infectious!L65,Deaths!L65)</f>
+        <v>618183</v>
+      </c>
+      <c r="M65" s="8" t="n">
+        <f aca="false">702972-SUM(Infectious!M65,Deaths!M65)</f>
+        <v>702703</v>
+      </c>
+      <c r="N65" s="8" t="n">
+        <f aca="false">781417-SUM(Infectious!N65,Deaths!N65)</f>
+        <v>781239</v>
+      </c>
+      <c r="O65" s="8" t="n">
+        <f aca="false">495955-SUM(Infectious!O65,Deaths!O65)</f>
+        <v>495762</v>
+      </c>
+      <c r="P65" s="8" t="n">
+        <f aca="false">69326-SUM(Infectious!P65,Deaths!P65)</f>
+        <v>69325</v>
+      </c>
+      <c r="Q65" s="8" t="n">
+        <f aca="false">457275-SUM(Infectious!Q65,Deaths!Q65)</f>
+        <v>457038</v>
+      </c>
+      <c r="R65" s="8" t="n">
+        <f aca="false">671252-SUM(Infectious!R65,Deaths!R65)</f>
+        <v>671019</v>
+      </c>
+      <c r="S65" s="8" t="n">
+        <f aca="false">539227-SUM(Infectious!S65,Deaths!S65)</f>
+        <v>538995</v>
+      </c>
+      <c r="T65" s="8" t="n">
+        <f aca="false">205329-SUM(Infectious!T65,Deaths!T65)</f>
+        <v>205132</v>
+      </c>
+      <c r="U65" s="8" t="n">
+        <f aca="false">162148-SUM(Infectious!U65,Deaths!U65)</f>
+        <v>162126</v>
+      </c>
+      <c r="V65" s="8" t="n">
+        <f aca="false">470393-SUM(Infectious!V65,Deaths!V65)</f>
+        <v>470169</v>
+      </c>
+      <c r="W65" s="8" t="n">
+        <f aca="false">478786-SUM(Infectious!W65,Deaths!W65)</f>
+        <v>478557</v>
+      </c>
+      <c r="X65" s="8" t="n">
+        <f aca="false">1161370-SUM(Infectious!X65,Deaths!X65)</f>
+        <v>1161064</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="n">
+        <v>44407</v>
+      </c>
+      <c r="B66" s="8" t="n">
+        <f aca="false">8926959 -SUM(Infectious!B66,Deaths!B66)</f>
+        <v>8923069</v>
+      </c>
+      <c r="C66" s="9" t="n">
+        <f aca="false">139485-SUM(Infectious!C66,Deaths!C66)</f>
+        <v>139435</v>
+      </c>
+      <c r="D66" s="8" t="n">
+        <f aca="false">189258--SUM(Infectious!D66,Deaths!D66)</f>
+        <v>189491</v>
+      </c>
+      <c r="E66" s="8" t="n">
+        <f aca="false">173970-SUM(Infectious!E66,Deaths!E66)</f>
+        <v>173696</v>
+      </c>
+      <c r="F66" s="8" t="n">
+        <f aca="false">157920-SUM(Infectious!F66,Deaths!F66)</f>
+        <v>157831</v>
+      </c>
+      <c r="G66" s="8" t="n">
+        <f aca="false">232077-SUM(Infectious!G66,Deaths!G66)</f>
+        <v>232044</v>
+      </c>
+      <c r="H66" s="8" t="n">
+        <f aca="false">356380-SUM(Infectious!H66,Deaths!H66)</f>
+        <v>355856</v>
+      </c>
+      <c r="I66" s="8" t="n">
+        <f aca="false">422151-SUM(Infectious!I66,Deaths!I66)</f>
+        <v>421990</v>
+      </c>
+      <c r="J66" s="8" t="n">
+        <f aca="false">233223-SUM(Infectious!J66,Deaths!J66)</f>
+        <v>233016</v>
+      </c>
+      <c r="K66" s="8" t="n">
+        <f aca="false">208680-SUM(Infectious!K66,Deaths!K66)</f>
+        <v>208486</v>
+      </c>
+      <c r="L66" s="8" t="n">
+        <f aca="false">618365-SUM(Infectious!L66,Deaths!L66)</f>
+        <v>618180</v>
+      </c>
+      <c r="M66" s="8" t="n">
+        <f aca="false">702972-SUM(Infectious!M66,Deaths!M66)</f>
+        <v>702517</v>
+      </c>
+      <c r="N66" s="8" t="n">
+        <f aca="false">781417-SUM(Infectious!N66,Deaths!N66)</f>
+        <v>781318</v>
+      </c>
+      <c r="O66" s="8" t="n">
+        <f aca="false">495955-SUM(Infectious!O66,Deaths!O66)</f>
+        <v>495780</v>
+      </c>
+      <c r="P66" s="8" t="n">
+        <f aca="false">69326-SUM(Infectious!P66,Deaths!P66)</f>
+        <v>69298</v>
+      </c>
+      <c r="Q66" s="8" t="n">
+        <f aca="false">457275-SUM(Infectious!Q66,Deaths!Q66)</f>
+        <v>457263</v>
+      </c>
+      <c r="R66" s="8" t="n">
+        <f aca="false">671252-SUM(Infectious!R66,Deaths!R66)</f>
+        <v>671090</v>
+      </c>
+      <c r="S66" s="8" t="n">
+        <f aca="false">539227-SUM(Infectious!S66,Deaths!S66)</f>
+        <v>539076</v>
+      </c>
+      <c r="T66" s="8" t="n">
+        <f aca="false">205329-SUM(Infectious!T66,Deaths!T66)</f>
+        <v>205097</v>
+      </c>
+      <c r="U66" s="8" t="n">
+        <f aca="false">162148-SUM(Infectious!U66,Deaths!U66)</f>
+        <v>162118</v>
+      </c>
+      <c r="V66" s="8" t="n">
+        <f aca="false">470393-SUM(Infectious!V66,Deaths!V66)</f>
+        <v>470284</v>
+      </c>
+      <c r="W66" s="8" t="n">
+        <f aca="false">478786-SUM(Infectious!W66,Deaths!W66)</f>
+        <v>478689</v>
+      </c>
+      <c r="X66" s="8" t="n">
+        <f aca="false">1161370-SUM(Infectious!X66,Deaths!X66)</f>
+        <v>1160980</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>

</xml_diff>

<commit_message>
fix day column in csv, e_day = e_acc//5
</commit_message>
<xml_diff>
--- a/COVID-19/HCM/SEIRD_data_12_7_2021.xlsx
+++ b/COVID-19/HCM/SEIRD_data_12_7_2021.xlsx
@@ -251,8 +251,8 @@
   </sheetPr>
   <dimension ref="A1:X83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76:X77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5977,17 +5977,305 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="80" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3"/>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="n">
+        <v>44419</v>
+      </c>
+      <c r="B78" s="5" t="n">
+        <f aca="false">SUM(C78:X78)</f>
+        <v>950</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="D78" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="F78" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G78" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="H78" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="I78" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="J78" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="K78" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="L78" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="M78" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="N78" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="O78" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="P78" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q78" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="R78" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="S78" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="T78" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="U78" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="V78" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="W78" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="X78" s="1" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="n">
+        <v>44420</v>
+      </c>
+      <c r="B79" s="5" t="n">
+        <f aca="false">SUM(C79:X79)</f>
+        <v>1361</v>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="D79" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="F79" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="G79" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="H79" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="I79" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="J79" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="K79" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="L79" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="M79" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="N79" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="O79" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="P79" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q79" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="R79" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="S79" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="T79" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="U79" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="V79" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="W79" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="X79" s="1" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="n">
+        <v>44421</v>
+      </c>
+      <c r="B80" s="5" t="n">
+        <f aca="false">SUM(C80:X80)</f>
+        <v>1214</v>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D80" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="F80" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G80" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="H80" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="I80" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="J80" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="K80" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="L80" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="M80" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="N80" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="O80" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="P80" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q80" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R80" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="S80" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="T80" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="U80" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="V80" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="W80" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="X80" s="1" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="n">
+        <v>44422</v>
+      </c>
+      <c r="B81" s="5" t="n">
+        <f aca="false">SUM(C81:X81)</f>
+        <v>1633</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="D81" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="F81" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="G81" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="H81" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="J81" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="K81" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="L81" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="M81" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="N81" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="O81" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="P81" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q81" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="R81" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="S81" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="T81" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="U81" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V81" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="W81" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="X81" s="1" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>
@@ -6013,8 +6301,8 @@
   </sheetPr>
   <dimension ref="A1:Z83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76:X77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11785,17 +12073,305 @@
         <v>156</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="80" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3"/>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="n">
+        <v>44419</v>
+      </c>
+      <c r="B78" s="1" t="n">
+        <f aca="false">SUM(C78:X78)</f>
+        <v>2378</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="D78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="F78" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="G78" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="H78" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="I78" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="J78" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="K78" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="L78" s="1" t="n">
+        <v>281</v>
+      </c>
+      <c r="M78" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="N78" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="O78" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="P78" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q78" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="R78" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="S78" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="T78" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="U78" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="V78" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="W78" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="X78" s="1" t="n">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="n">
+        <v>44420</v>
+      </c>
+      <c r="B79" s="1" t="n">
+        <f aca="false">SUM(C79:X79)</f>
+        <v>2420</v>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="D79" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="F79" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="G79" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="H79" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="I79" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="J79" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="K79" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="L79" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="M79" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="N79" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="O79" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="P79" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q79" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="R79" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="S79" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="T79" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="U79" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="V79" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="W79" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="X79" s="1" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="n">
+        <v>44421</v>
+      </c>
+      <c r="B80" s="1" t="n">
+        <f aca="false">SUM(C80:X80)</f>
+        <v>2278</v>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="D80" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="F80" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="G80" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="H80" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="I80" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="J80" s="1" t="n">
+        <v>311</v>
+      </c>
+      <c r="K80" s="1" t="n">
+        <v>309</v>
+      </c>
+      <c r="L80" s="1" t="n">
+        <v>243</v>
+      </c>
+      <c r="M80" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="N80" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="O80" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="P80" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q80" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="R80" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="S80" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="T80" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="U80" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="V80" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="W80" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="X80" s="1" t="n">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="n">
+        <v>44422</v>
+      </c>
+      <c r="B81" s="1" t="n">
+        <f aca="false">SUM(C81:X81)</f>
+        <v>2542</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="D81" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F81" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="G81" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H81" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="J81" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="K81" s="1" t="n">
+        <v>276</v>
+      </c>
+      <c r="L81" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="M81" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="N81" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="O81" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="P81" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q81" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="R81" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="S81" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="T81" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="U81" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="V81" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="W81" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="X81" s="1" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>
@@ -11819,13 +12395,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y77"/>
+  <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q48" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76:X77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="9.78"/>
@@ -18799,11 +19375,11 @@
         <v>44414</v>
       </c>
       <c r="B73" s="5" t="n">
-        <v>2821</v>
+        <v>2823</v>
       </c>
       <c r="C73" s="8" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C73+Exposed!C73)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D73" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D73+Exposed!D73)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -18827,7 +19403,7 @@
       </c>
       <c r="I73" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I73+Exposed!I73)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="J73" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J73+Exposed!J73)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -18896,95 +19472,95 @@
         <v>44415</v>
       </c>
       <c r="B74" s="5" t="n">
-        <v>2822</v>
+        <v>3333</v>
       </c>
       <c r="C74" s="8" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C74+Exposed!C74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D74" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D74+Exposed!D74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="E74" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E74+Exposed!E74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="F74" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F74+Exposed!F74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G74" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G74+Exposed!G74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="H74" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H74+Exposed!H74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="I74" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I74+Exposed!I74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>290</v>
+        <v>343</v>
       </c>
       <c r="J74" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J74+Exposed!J74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>233</v>
+        <v>275</v>
       </c>
       <c r="K74" s="5" t="n">
         <f aca="true" t="array" ref="K74:K74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K74+Exposed!K74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="L74" s="5" t="n">
         <f aca="true" t="array" ref="L74:L74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L74+Exposed!L74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>215</v>
+        <v>254</v>
       </c>
       <c r="M74" s="5" t="n">
         <f aca="true" t="array" ref="M74:M74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M74+Exposed!M74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="N74" s="5" t="n">
         <f aca="true" t="array" ref="N74:N74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N74+Exposed!N74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="O74" s="5" t="n">
         <f aca="true" t="array" ref="O74:O74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O74+Exposed!O74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>291</v>
+        <v>344</v>
       </c>
       <c r="P74" s="5" t="n">
         <f aca="true" t="array" ref="P74:P74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P74+Exposed!P74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="Q74" s="5" t="n">
         <f aca="true" t="array" ref="Q74:Q74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q74+Exposed!Q74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="R74" s="5" t="n">
         <f aca="true" t="array" ref="R74:R74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R74+Exposed!R74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="S74" s="5" t="n">
         <f aca="true" t="array" ref="S74:S74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S74+Exposed!S74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="T74" s="5" t="n">
         <f aca="true" t="array" ref="T74:T74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T74+Exposed!T74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="U74" s="5" t="n">
         <f aca="true" t="array" ref="U74:U74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U74+Exposed!U74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="V74" s="5" t="n">
         <f aca="true" t="array" ref="V74:V74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V74+Exposed!V74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="W74" s="5" t="n">
         <f aca="true" t="array" ref="W74:W74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W74+Exposed!W74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="X74" s="5" t="n">
         <f aca="true" t="array" ref="X74:X74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X74+Exposed!X74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>298</v>
+        <v>352</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19088,95 +19664,95 @@
         <v>44417</v>
       </c>
       <c r="B76" s="5" t="n">
-        <v>2824</v>
+        <v>2206</v>
       </c>
       <c r="C76" s="8" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C76+Exposed!C76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="D76" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D76+Exposed!D76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E76" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E76+Exposed!E76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="F76" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F76+Exposed!F76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>224</v>
+        <v>175</v>
       </c>
       <c r="G76" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G76+Exposed!G76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="H76" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H76+Exposed!H76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="I76" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I76+Exposed!I76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>489</v>
+        <v>382</v>
       </c>
       <c r="J76" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J76+Exposed!J76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>233</v>
+        <v>182</v>
       </c>
       <c r="K76" s="5" t="n">
         <f aca="true" t="array" ref="K76:K76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K76+Exposed!K76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="L76" s="5" t="n">
         <f aca="true" t="array" ref="L76:L76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L76+Exposed!L76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="M76" s="5" t="n">
         <f aca="true" t="array" ref="M76:M76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M76+Exposed!M76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="N76" s="5" t="n">
         <f aca="true" t="array" ref="N76:N76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N76+Exposed!N76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="O76" s="5" t="n">
         <f aca="true" t="array" ref="O76:O76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O76+Exposed!O76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>215</v>
+        <v>168</v>
       </c>
       <c r="P76" s="5" t="n">
         <f aca="true" t="array" ref="P76:P76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P76+Exposed!P76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="Q76" s="5" t="n">
         <f aca="true" t="array" ref="Q76:Q76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q76+Exposed!Q76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="R76" s="5" t="n">
         <f aca="true" t="array" ref="R76:R76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R76+Exposed!R76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="S76" s="5" t="n">
         <f aca="true" t="array" ref="S76:S76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S76+Exposed!S76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="T76" s="5" t="n">
         <f aca="true" t="array" ref="T76:T76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T76+Exposed!T76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="U76" s="5" t="n">
         <f aca="true" t="array" ref="U76:U76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U76+Exposed!U76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="V76" s="5" t="n">
         <f aca="true" t="array" ref="V76:V76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V76+Exposed!V76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="W76" s="5" t="n">
         <f aca="true" t="array" ref="W76:W76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W76+Exposed!W76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="X76" s="5" t="n">
         <f aca="true" t="array" ref="X76:X76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X76+Exposed!X76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19184,97 +19760,482 @@
         <v>44418</v>
       </c>
       <c r="B77" s="5" t="n">
-        <v>2825</v>
+        <v>2964</v>
       </c>
       <c r="C77" s="8" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C77+Exposed!C77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="D77" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D77+Exposed!D77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="E77" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E77+Exposed!E77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="F77" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F77+Exposed!F77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="G77" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G77+Exposed!G77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H77" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H77+Exposed!H77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I77" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I77+Exposed!I77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="J77" s="5" t="n">
         <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J77+Exposed!J77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K77" s="5" t="n">
         <f aca="true" t="array" ref="K77:K77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K77+Exposed!K77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="L77" s="5" t="n">
         <f aca="true" t="array" ref="L77:L77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L77+Exposed!L77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="M77" s="5" t="n">
         <f aca="true" t="array" ref="M77:M77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M77+Exposed!M77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="N77" s="5" t="n">
         <f aca="true" t="array" ref="N77:N77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N77+Exposed!N77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="O77" s="5" t="n">
         <f aca="true" t="array" ref="O77:O77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O77+Exposed!O77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="P77" s="5" t="n">
         <f aca="true" t="array" ref="P77:P77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P77+Exposed!P77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q77" s="5" t="n">
         <f aca="true" t="array" ref="Q77:Q77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q77+Exposed!Q77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="R77" s="5" t="n">
         <f aca="true" t="array" ref="R77:R77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R77+Exposed!R77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="S77" s="5" t="n">
         <f aca="true" t="array" ref="S77:S77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S77+Exposed!S77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="T77" s="5" t="n">
         <f aca="true" t="array" ref="T77:T77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T77+Exposed!T77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="U77" s="5" t="n">
         <f aca="true" t="array" ref="U77:U77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U77+Exposed!U77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="V77" s="5" t="n">
         <f aca="true" t="array" ref="V77:V77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V77+Exposed!V77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="W77" s="5" t="n">
         <f aca="true" t="array" ref="W77:W77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W77+Exposed!W77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="X77" s="5" t="n">
         <f aca="true" t="array" ref="X77:X77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X77+Exposed!X77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="7" t="n">
+        <v>44419</v>
+      </c>
+      <c r="B78" s="5" t="n">
+        <v>2042</v>
+      </c>
+      <c r="C78" s="8" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C78+Exposed!C78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>42</v>
+      </c>
+      <c r="D78" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D78+Exposed!D78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>87</v>
+      </c>
+      <c r="E78" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E78+Exposed!E78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>129</v>
+      </c>
+      <c r="F78" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F78+Exposed!F78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>31</v>
+      </c>
+      <c r="G78" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G78+Exposed!G78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>58</v>
+      </c>
+      <c r="H78" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H78+Exposed!H78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>45</v>
+      </c>
+      <c r="I78" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I78+Exposed!I78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>198</v>
+      </c>
+      <c r="J78" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J78+Exposed!J78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>148</v>
+      </c>
+      <c r="K78" s="5" t="n">
+        <f aca="true" t="array" ref="K78:K78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K78+Exposed!K78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>133</v>
+      </c>
+      <c r="L78" s="5" t="n">
+        <f aca="true" t="array" ref="L78:L78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L78+Exposed!L78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>183</v>
+      </c>
+      <c r="M78" s="5" t="n">
+        <f aca="true" t="array" ref="M78:M78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M78+Exposed!M78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>52</v>
+      </c>
+      <c r="N78" s="5" t="n">
+        <f aca="true" t="array" ref="N78:N78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N78+Exposed!N78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>90</v>
+      </c>
+      <c r="O78" s="5" t="n">
+        <f aca="true" t="array" ref="O78:O78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O78+Exposed!O78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>201</v>
+      </c>
+      <c r="P78" s="5" t="n">
+        <f aca="true" t="array" ref="P78:P78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P78+Exposed!P78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>13</v>
+      </c>
+      <c r="Q78" s="5" t="n">
+        <f aca="true" t="array" ref="Q78:Q78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q78+Exposed!Q78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>118</v>
+      </c>
+      <c r="R78" s="5" t="n">
+        <f aca="true" t="array" ref="R78:R78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R78+Exposed!R78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>84</v>
+      </c>
+      <c r="S78" s="5" t="n">
+        <f aca="true" t="array" ref="S78:S78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S78+Exposed!S78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>77</v>
+      </c>
+      <c r="T78" s="5" t="n">
+        <f aca="true" t="array" ref="T78:T78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T78+Exposed!T78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>33</v>
+      </c>
+      <c r="U78" s="5" t="n">
+        <f aca="true" t="array" ref="U78:U78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U78+Exposed!U78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>6</v>
+      </c>
+      <c r="V78" s="5" t="n">
+        <f aca="true" t="array" ref="V78:V78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V78+Exposed!V78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>83</v>
+      </c>
+      <c r="W78" s="5" t="n">
+        <f aca="true" t="array" ref="W78:W78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W78+Exposed!W78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>101</v>
+      </c>
+      <c r="X78" s="5" t="n">
+        <f aca="true" t="array" ref="X78:X78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X78+Exposed!X78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
         <v>131</v>
       </c>
     </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="7" t="n">
+        <v>44420</v>
+      </c>
+      <c r="B79" s="5" t="n">
+        <v>2149</v>
+      </c>
+      <c r="C79" s="8" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C79+Exposed!C79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>101</v>
+      </c>
+      <c r="D79" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D79+Exposed!D79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>102</v>
+      </c>
+      <c r="E79" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E79+Exposed!E79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>132</v>
+      </c>
+      <c r="F79" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F79+Exposed!F79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>75</v>
+      </c>
+      <c r="G79" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G79+Exposed!G79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>61</v>
+      </c>
+      <c r="H79" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H79+Exposed!H79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>33</v>
+      </c>
+      <c r="I79" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I79+Exposed!I79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>202</v>
+      </c>
+      <c r="J79" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J79+Exposed!J79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>30</v>
+      </c>
+      <c r="K79" s="5" t="n">
+        <f aca="true" t="array" ref="K79:K79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K79+Exposed!K79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>129</v>
+      </c>
+      <c r="L79" s="5" t="n">
+        <f aca="true" t="array" ref="L79:L79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L79+Exposed!L79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>131</v>
+      </c>
+      <c r="M79" s="5" t="n">
+        <f aca="true" t="array" ref="M79:M79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M79+Exposed!M79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>47</v>
+      </c>
+      <c r="N79" s="5" t="n">
+        <f aca="true" t="array" ref="N79:N79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N79+Exposed!N79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>136</v>
+      </c>
+      <c r="O79" s="5" t="n">
+        <f aca="true" t="array" ref="O79:O79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O79+Exposed!O79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>139</v>
+      </c>
+      <c r="P79" s="5" t="n">
+        <f aca="true" t="array" ref="P79:P79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P79+Exposed!P79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>9</v>
+      </c>
+      <c r="Q79" s="5" t="n">
+        <f aca="true" t="array" ref="Q79:Q79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q79+Exposed!Q79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>174</v>
+      </c>
+      <c r="R79" s="5" t="n">
+        <f aca="true" t="array" ref="R79:R79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R79+Exposed!R79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>45</v>
+      </c>
+      <c r="S79" s="5" t="n">
+        <f aca="true" t="array" ref="S79:S79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S79+Exposed!S79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>98</v>
+      </c>
+      <c r="T79" s="5" t="n">
+        <f aca="true" t="array" ref="T79:T79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T79+Exposed!T79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>164</v>
+      </c>
+      <c r="U79" s="5" t="n">
+        <f aca="true" t="array" ref="U79:U79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U79+Exposed!U79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>77</v>
+      </c>
+      <c r="V79" s="5" t="n">
+        <f aca="true" t="array" ref="V79:V79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V79+Exposed!V79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>89</v>
+      </c>
+      <c r="W79" s="5" t="n">
+        <f aca="true" t="array" ref="W79:W79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W79+Exposed!W79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>107</v>
+      </c>
+      <c r="X79" s="5" t="n">
+        <f aca="true" t="array" ref="X79:X79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X79+Exposed!X79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="7" t="n">
+        <v>44421</v>
+      </c>
+      <c r="B80" s="5" t="n">
+        <v>2175</v>
+      </c>
+      <c r="C80" s="8" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C80+Exposed!C80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>145</v>
+      </c>
+      <c r="D80" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D80+Exposed!D80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>58</v>
+      </c>
+      <c r="E80" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E80+Exposed!E80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>98</v>
+      </c>
+      <c r="F80" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F80+Exposed!F80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>59</v>
+      </c>
+      <c r="G80" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G80+Exposed!G80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>56</v>
+      </c>
+      <c r="H80" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H80+Exposed!H80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>44</v>
+      </c>
+      <c r="I80" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I80+Exposed!I80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>135</v>
+      </c>
+      <c r="J80" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J80+Exposed!J80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>219</v>
+      </c>
+      <c r="K80" s="5" t="n">
+        <f aca="true" t="array" ref="K80:K80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K80+Exposed!K80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>215</v>
+      </c>
+      <c r="L80" s="5" t="n">
+        <f aca="true" t="array" ref="L80:L80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L80+Exposed!L80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>166</v>
+      </c>
+      <c r="M80" s="5" t="n">
+        <f aca="true" t="array" ref="M80:M80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M80+Exposed!M80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>49</v>
+      </c>
+      <c r="N80" s="5" t="n">
+        <f aca="true" t="array" ref="N80:N80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N80+Exposed!N80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>90</v>
+      </c>
+      <c r="O80" s="5" t="n">
+        <f aca="true" t="array" ref="O80:O80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O80+Exposed!O80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>146</v>
+      </c>
+      <c r="P80" s="5" t="n">
+        <f aca="true" t="array" ref="P80:P80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P80+Exposed!P80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>18</v>
+      </c>
+      <c r="Q80" s="5" t="n">
+        <f aca="true" t="array" ref="Q80:Q80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q80+Exposed!Q80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>31</v>
+      </c>
+      <c r="R80" s="5" t="n">
+        <f aca="true" t="array" ref="R80:R80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R80+Exposed!R80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>92</v>
+      </c>
+      <c r="S80" s="5" t="n">
+        <f aca="true" t="array" ref="S80:S80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S80+Exposed!S80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>108</v>
+      </c>
+      <c r="T80" s="5" t="n">
+        <f aca="true" t="array" ref="T80:T80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T80+Exposed!T80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>27</v>
+      </c>
+      <c r="U80" s="5" t="n">
+        <f aca="true" t="array" ref="U80:U80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U80+Exposed!U80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>16</v>
+      </c>
+      <c r="V80" s="5" t="n">
+        <f aca="true" t="array" ref="V80:V80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V80+Exposed!V80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>171</v>
+      </c>
+      <c r="W80" s="5" t="n">
+        <f aca="true" t="array" ref="W80:W80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W80+Exposed!W80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>111</v>
+      </c>
+      <c r="X80" s="5" t="n">
+        <f aca="true" t="array" ref="X80:X80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X80+Exposed!X80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="7" t="n">
+        <v>44422</v>
+      </c>
+      <c r="B81" s="5" t="n">
+        <v>3417</v>
+      </c>
+      <c r="C81" s="8" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C81+Exposed!C81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>135</v>
+      </c>
+      <c r="D81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D81+Exposed!D81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>303</v>
+      </c>
+      <c r="E81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E81+Exposed!E81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>128</v>
+      </c>
+      <c r="F81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F81+Exposed!F81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>228</v>
+      </c>
+      <c r="G81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G81+Exposed!G81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>90</v>
+      </c>
+      <c r="H81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H81+Exposed!H81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>52</v>
+      </c>
+      <c r="I81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I81+Exposed!I81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>190</v>
+      </c>
+      <c r="J81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J81+Exposed!J81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>162</v>
+      </c>
+      <c r="K81" s="5" t="n">
+        <f aca="true" t="array" ref="K81:K81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K81+Exposed!K81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>269</v>
+      </c>
+      <c r="L81" s="5" t="n">
+        <f aca="true" t="array" ref="L81:L81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L81+Exposed!L81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>66</v>
+      </c>
+      <c r="M81" s="5" t="n">
+        <f aca="true" t="array" ref="M81:M81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M81+Exposed!M81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>88</v>
+      </c>
+      <c r="N81" s="5" t="n">
+        <f aca="true" t="array" ref="N81:N81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N81+Exposed!N81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>305</v>
+      </c>
+      <c r="O81" s="5" t="n">
+        <f aca="true" t="array" ref="O81:O81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O81+Exposed!O81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>209</v>
+      </c>
+      <c r="P81" s="5" t="n">
+        <f aca="true" t="array" ref="P81:P81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P81+Exposed!P81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>29</v>
+      </c>
+      <c r="Q81" s="5" t="n">
+        <f aca="true" t="array" ref="Q81:Q81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q81+Exposed!Q81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>179</v>
+      </c>
+      <c r="R81" s="5" t="n">
+        <f aca="true" t="array" ref="R81:R81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R81+Exposed!R81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>83</v>
+      </c>
+      <c r="S81" s="5" t="n">
+        <f aca="true" t="array" ref="S81:S81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S81+Exposed!S81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>94</v>
+      </c>
+      <c r="T81" s="5" t="n">
+        <f aca="true" t="array" ref="T81:T81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T81+Exposed!T81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>210</v>
+      </c>
+      <c r="U81" s="5" t="n">
+        <f aca="true" t="array" ref="U81:U81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U81+Exposed!U81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>71</v>
+      </c>
+      <c r="V81" s="5" t="n">
+        <f aca="true" t="array" ref="V81:V81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V81+Exposed!V81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>257</v>
+      </c>
+      <c r="W81" s="5" t="n">
+        <f aca="true" t="array" ref="W81:W81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W81+Exposed!W81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>115</v>
+      </c>
+      <c r="X81" s="5" t="n">
+        <f aca="true" t="array" ref="X81:X81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X81+Exposed!X81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -19293,11 +20254,11 @@
   </sheetPr>
   <dimension ref="A1:X82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q56" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76:X77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B81" activeCellId="0" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="1" width="11.57"/>
   </cols>
@@ -26197,7 +27158,7 @@
         <v>44414</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C73" s="1" t="n">
         <f aca="true" t="array" ref="C73:C73">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C73+Exposed!C73)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26229,7 +27190,7 @@
       </c>
       <c r="J73" s="1" t="n">
         <f aca="true" t="array" ref="J73:J73">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J73+Exposed!J73)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K73" s="1" t="n">
         <f aca="true" t="array" ref="K73:K73">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K73+Exposed!K73)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26293,63 +27254,63 @@
         <v>44415</v>
       </c>
       <c r="B74" s="1" t="n">
-        <v>221</v>
+        <v>185</v>
       </c>
       <c r="C74" s="1" t="n">
         <f aca="true" t="array" ref="C74:C74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C74+Exposed!C74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D74" s="1" t="n">
         <f aca="true" t="array" ref="D74:D74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D74+Exposed!D74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E74" s="1" t="n">
         <f aca="true" t="array" ref="E74:E74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E74+Exposed!E74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" s="1" t="n">
         <f aca="true" t="array" ref="F74:F74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F74+Exposed!F74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G74" s="1" t="n">
         <f aca="true" t="array" ref="G74:G74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G74+Exposed!G74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H74" s="1" t="n">
         <f aca="true" t="array" ref="H74:H74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H74+Exposed!H74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I74" s="1" t="n">
         <f aca="true" t="array" ref="I74:I74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I74+Exposed!I74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J74" s="1" t="n">
         <f aca="true" t="array" ref="J74:J74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J74+Exposed!J74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K74" s="1" t="n">
         <f aca="true" t="array" ref="K74:K74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K74+Exposed!K74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L74" s="1" t="n">
         <f aca="true" t="array" ref="L74:L74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L74+Exposed!L74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M74" s="1" t="n">
         <f aca="true" t="array" ref="M74:M74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M74+Exposed!M74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N74" s="1" t="n">
         <f aca="true" t="array" ref="N74:N74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N74+Exposed!N74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O74" s="1" t="n">
         <f aca="true" t="array" ref="O74:O74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O74+Exposed!O74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="P74" s="1" t="n">
         <f aca="true" t="array" ref="P74:P74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P74+Exposed!P74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q74" s="1" t="n">
         <f aca="true" t="array" ref="Q74:Q74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q74+Exposed!Q74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26357,15 +27318,15 @@
       </c>
       <c r="R74" s="1" t="n">
         <f aca="true" t="array" ref="R74:R74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R74+Exposed!R74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S74" s="1" t="n">
         <f aca="true" t="array" ref="S74:S74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S74+Exposed!S74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T74" s="1" t="n">
         <f aca="true" t="array" ref="T74:T74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T74+Exposed!T74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="U74" s="1" t="n">
         <f aca="true" t="array" ref="U74:U74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U74+Exposed!U74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26373,15 +27334,15 @@
       </c>
       <c r="V74" s="1" t="n">
         <f aca="true" t="array" ref="V74:V74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V74+Exposed!V74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W74" s="1" t="n">
         <f aca="true" t="array" ref="W74:W74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W74+Exposed!W74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="X74" s="1" t="n">
         <f aca="true" t="array" ref="X74:X74">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X74+Exposed!X74)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26389,11 +27350,11 @@
         <v>44416</v>
       </c>
       <c r="B75" s="1" t="n">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="C75" s="1" t="n">
         <f aca="true" t="array" ref="C75:C75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C75+Exposed!C75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D75" s="1" t="n">
         <f aca="true" t="array" ref="D75:D75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D75+Exposed!D75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26405,7 +27366,7 @@
       </c>
       <c r="F75" s="1" t="n">
         <f aca="true" t="array" ref="F75:F75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F75+Exposed!F75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G75" s="1" t="n">
         <f aca="true" t="array" ref="G75:G75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G75+Exposed!G75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26417,11 +27378,11 @@
       </c>
       <c r="I75" s="1" t="n">
         <f aca="true" t="array" ref="I75:I75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I75+Exposed!I75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J75" s="1" t="n">
         <f aca="true" t="array" ref="J75:J75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J75+Exposed!J75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K75" s="1" t="n">
         <f aca="true" t="array" ref="K75:K75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K75+Exposed!K75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26429,11 +27390,11 @@
       </c>
       <c r="L75" s="1" t="n">
         <f aca="true" t="array" ref="L75:L75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L75+Exposed!L75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M75" s="1" t="n">
         <f aca="true" t="array" ref="M75:M75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M75+Exposed!M75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N75" s="1" t="n">
         <f aca="true" t="array" ref="N75:N75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N75+Exposed!N75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26441,7 +27402,7 @@
       </c>
       <c r="O75" s="1" t="n">
         <f aca="true" t="array" ref="O75:O75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O75+Exposed!O75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P75" s="1" t="n">
         <f aca="true" t="array" ref="P75:P75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P75+Exposed!P75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26453,11 +27414,11 @@
       </c>
       <c r="R75" s="1" t="n">
         <f aca="true" t="array" ref="R75:R75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R75+Exposed!R75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S75" s="1" t="n">
         <f aca="true" t="array" ref="S75:S75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S75+Exposed!S75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T75" s="1" t="n">
         <f aca="true" t="array" ref="T75:T75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T75+Exposed!T75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26473,7 +27434,7 @@
       </c>
       <c r="W75" s="1" t="n">
         <f aca="true" t="array" ref="W75:W75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W75+Exposed!W75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="X75" s="1" t="n">
         <f aca="true" t="array" ref="X75:X75">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X75+Exposed!X75)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26485,27 +27446,27 @@
         <v>44417</v>
       </c>
       <c r="B76" s="1" t="n">
-        <v>223</v>
+        <v>269</v>
       </c>
       <c r="C76" s="1" t="n">
         <f aca="true" t="array" ref="C76:C76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C76+Exposed!C76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D76" s="1" t="n">
         <f aca="true" t="array" ref="D76:D76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D76+Exposed!D76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E76" s="1" t="n">
         <f aca="true" t="array" ref="E76:E76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E76+Exposed!E76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F76" s="1" t="n">
         <f aca="true" t="array" ref="F76:F76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F76+Exposed!F76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G76" s="1" t="n">
         <f aca="true" t="array" ref="G76:G76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G76+Exposed!G76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H76" s="1" t="n">
         <f aca="true" t="array" ref="H76:H76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H76+Exposed!H76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26513,51 +27474,51 @@
       </c>
       <c r="I76" s="1" t="n">
         <f aca="true" t="array" ref="I76:I76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I76+Exposed!I76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="J76" s="1" t="n">
         <f aca="true" t="array" ref="J76:J76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J76+Exposed!J76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K76" s="1" t="n">
         <f aca="true" t="array" ref="K76:K76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K76+Exposed!K76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L76" s="1" t="n">
         <f aca="true" t="array" ref="L76:L76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L76+Exposed!L76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M76" s="1" t="n">
         <f aca="true" t="array" ref="M76:M76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M76+Exposed!M76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N76" s="1" t="n">
         <f aca="true" t="array" ref="N76:N76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N76+Exposed!N76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O76" s="1" t="n">
         <f aca="true" t="array" ref="O76:O76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O76+Exposed!O76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="P76" s="1" t="n">
         <f aca="true" t="array" ref="P76:P76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P76+Exposed!P76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q76" s="1" t="n">
         <f aca="true" t="array" ref="Q76:Q76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q76+Exposed!Q76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="R76" s="1" t="n">
         <f aca="true" t="array" ref="R76:R76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R76+Exposed!R76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="S76" s="1" t="n">
         <f aca="true" t="array" ref="S76:S76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S76+Exposed!S76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="T76" s="1" t="n">
         <f aca="true" t="array" ref="T76:T76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T76+Exposed!T76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U76" s="1" t="n">
         <f aca="true" t="array" ref="U76:U76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U76+Exposed!U76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
@@ -26565,15 +27526,15 @@
       </c>
       <c r="V76" s="1" t="n">
         <f aca="true" t="array" ref="V76:V76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V76+Exposed!V76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="W76" s="1" t="n">
         <f aca="true" t="array" ref="W76:W76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W76+Exposed!W76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X76" s="1" t="n">
         <f aca="true" t="array" ref="X76:X76">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X76+Exposed!X76)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26581,108 +27542,480 @@
         <v>44418</v>
       </c>
       <c r="B77" s="1" t="n">
-        <v>224</v>
+        <v>308</v>
       </c>
       <c r="C77" s="1" t="n">
         <f aca="true" t="array" ref="C77:C77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C77+Exposed!C77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D77" s="1" t="n">
         <f aca="true" t="array" ref="D77:D77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D77+Exposed!D77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E77" s="1" t="n">
         <f aca="true" t="array" ref="E77:E77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E77+Exposed!E77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F77" s="1" t="n">
         <f aca="true" t="array" ref="F77:F77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F77+Exposed!F77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G77" s="1" t="n">
         <f aca="true" t="array" ref="G77:G77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G77+Exposed!G77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H77" s="1" t="n">
         <f aca="true" t="array" ref="H77:H77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H77+Exposed!H77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I77" s="1" t="n">
         <f aca="true" t="array" ref="I77:I77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I77+Exposed!I77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J77" s="1" t="n">
         <f aca="true" t="array" ref="J77:J77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J77+Exposed!J77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K77" s="1" t="n">
         <f aca="true" t="array" ref="K77:K77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K77+Exposed!K77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L77" s="1" t="n">
         <f aca="true" t="array" ref="L77:L77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L77+Exposed!L77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="M77" s="1" t="n">
         <f aca="true" t="array" ref="M77:M77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M77+Exposed!M77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N77" s="1" t="n">
         <f aca="true" t="array" ref="N77:N77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N77+Exposed!N77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="O77" s="1" t="n">
         <f aca="true" t="array" ref="O77:O77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O77+Exposed!O77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="P77" s="1" t="n">
         <f aca="true" t="array" ref="P77:P77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P77+Exposed!P77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q77" s="1" t="n">
         <f aca="true" t="array" ref="Q77:Q77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q77+Exposed!Q77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R77" s="1" t="n">
         <f aca="true" t="array" ref="R77:R77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R77+Exposed!R77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="S77" s="1" t="n">
         <f aca="true" t="array" ref="S77:S77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S77+Exposed!S77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="T77" s="1" t="n">
         <f aca="true" t="array" ref="T77:T77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T77+Exposed!T77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U77" s="1" t="n">
         <f aca="true" t="array" ref="U77:U77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U77+Exposed!U77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="V77" s="1" t="n">
         <f aca="true" t="array" ref="V77:V77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V77+Exposed!V77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="W77" s="1" t="n">
         <f aca="true" t="array" ref="W77:W77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W77+Exposed!W77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="X77" s="1" t="n">
         <f aca="true" t="array" ref="X77:X77">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X77+Exposed!X77)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="n">
+        <v>44419</v>
+      </c>
+      <c r="B78" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <f aca="true" t="array" ref="C78:C78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C78+Exposed!C78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>5</v>
+      </c>
+      <c r="D78" s="1" t="n">
+        <f aca="true" t="array" ref="D78:D78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D78+Exposed!D78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <f aca="true" t="array" ref="E78:E78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E78+Exposed!E78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>17</v>
+      </c>
+      <c r="F78" s="1" t="n">
+        <f aca="true" t="array" ref="F78:F78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F78+Exposed!F78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>4</v>
+      </c>
+      <c r="G78" s="1" t="n">
+        <f aca="true" t="array" ref="G78:G78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G78+Exposed!G78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>7</v>
+      </c>
+      <c r="H78" s="1" t="n">
+        <f aca="true" t="array" ref="H78:H78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H78+Exposed!H78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>6</v>
+      </c>
+      <c r="I78" s="1" t="n">
+        <f aca="true" t="array" ref="I78:I78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I78+Exposed!I78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>25</v>
+      </c>
+      <c r="J78" s="1" t="n">
+        <f aca="true" t="array" ref="J78:J78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J78+Exposed!J78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>19</v>
+      </c>
+      <c r="K78" s="1" t="n">
+        <f aca="true" t="array" ref="K78:K78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K78+Exposed!K78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>17</v>
+      </c>
+      <c r="L78" s="1" t="n">
+        <f aca="true" t="array" ref="L78:L78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L78+Exposed!L78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>23</v>
+      </c>
+      <c r="M78" s="1" t="n">
+        <f aca="true" t="array" ref="M78:M78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M78+Exposed!M78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>7</v>
+      </c>
+      <c r="N78" s="1" t="n">
+        <f aca="true" t="array" ref="N78:N78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N78+Exposed!N78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="O78" s="1" t="n">
+        <f aca="true" t="array" ref="O78:O78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O78+Exposed!O78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>26</v>
+      </c>
+      <c r="P78" s="1" t="n">
+        <f aca="true" t="array" ref="P78:P78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P78+Exposed!P78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>2</v>
+      </c>
+      <c r="Q78" s="1" t="n">
+        <f aca="true" t="array" ref="Q78:Q78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q78+Exposed!Q78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>15</v>
+      </c>
+      <c r="R78" s="1" t="n">
+        <f aca="true" t="array" ref="R78:R78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R78+Exposed!R78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="S78" s="1" t="n">
+        <f aca="true" t="array" ref="S78:S78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S78+Exposed!S78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="80" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3"/>
+      <c r="T78" s="1" t="n">
+        <f aca="true" t="array" ref="T78:T78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T78+Exposed!T78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>4</v>
+      </c>
+      <c r="U78" s="1" t="n">
+        <f aca="true" t="array" ref="U78:U78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U78+Exposed!U78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>1</v>
+      </c>
+      <c r="V78" s="1" t="n">
+        <f aca="true" t="array" ref="V78:V78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V78+Exposed!V78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="W78" s="1" t="n">
+        <f aca="true" t="array" ref="W78:W78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W78+Exposed!W78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>13</v>
+      </c>
+      <c r="X78" s="1" t="n">
+        <f aca="true" t="array" ref="X78:X78">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X78+Exposed!X78)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="n">
+        <v>44420</v>
+      </c>
+      <c r="B79" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="C79" s="1" t="n">
+        <f aca="true" t="array" ref="C79:C79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C79+Exposed!C79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="D79" s="1" t="n">
+        <f aca="true" t="array" ref="D79:D79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D79+Exposed!D79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <f aca="true" t="array" ref="E79:E79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E79+Exposed!E79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>14</v>
+      </c>
+      <c r="F79" s="1" t="n">
+        <f aca="true" t="array" ref="F79:F79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F79+Exposed!F79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>8</v>
+      </c>
+      <c r="G79" s="1" t="n">
+        <f aca="true" t="array" ref="G79:G79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G79+Exposed!G79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>6</v>
+      </c>
+      <c r="H79" s="1" t="n">
+        <f aca="true" t="array" ref="H79:H79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H79+Exposed!H79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>3</v>
+      </c>
+      <c r="I79" s="1" t="n">
+        <f aca="true" t="array" ref="I79:I79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I79+Exposed!I79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>21</v>
+      </c>
+      <c r="J79" s="1" t="n">
+        <f aca="true" t="array" ref="J79:J79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J79+Exposed!J79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>3</v>
+      </c>
+      <c r="K79" s="1" t="n">
+        <f aca="true" t="array" ref="K79:K79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K79+Exposed!K79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>14</v>
+      </c>
+      <c r="L79" s="1" t="n">
+        <f aca="true" t="array" ref="L79:L79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L79+Exposed!L79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>14</v>
+      </c>
+      <c r="M79" s="1" t="n">
+        <f aca="true" t="array" ref="M79:M79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M79+Exposed!M79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>5</v>
+      </c>
+      <c r="N79" s="1" t="n">
+        <f aca="true" t="array" ref="N79:N79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N79+Exposed!N79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>14</v>
+      </c>
+      <c r="O79" s="1" t="n">
+        <f aca="true" t="array" ref="O79:O79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O79+Exposed!O79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>15</v>
+      </c>
+      <c r="P79" s="1" t="n">
+        <f aca="true" t="array" ref="P79:P79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P79+Exposed!P79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q79" s="1" t="n">
+        <f aca="true" t="array" ref="Q79:Q79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q79+Exposed!Q79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>18</v>
+      </c>
+      <c r="R79" s="1" t="n">
+        <f aca="true" t="array" ref="R79:R79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R79+Exposed!R79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>5</v>
+      </c>
+      <c r="S79" s="1" t="n">
+        <f aca="true" t="array" ref="S79:S79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S79+Exposed!S79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>10</v>
+      </c>
+      <c r="T79" s="1" t="n">
+        <f aca="true" t="array" ref="T79:T79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T79+Exposed!T79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>17</v>
+      </c>
+      <c r="U79" s="1" t="n">
+        <f aca="true" t="array" ref="U79:U79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U79+Exposed!U79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>8</v>
+      </c>
+      <c r="V79" s="1" t="n">
+        <f aca="true" t="array" ref="V79:V79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V79+Exposed!V79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>9</v>
+      </c>
+      <c r="W79" s="1" t="n">
+        <f aca="true" t="array" ref="W79:W79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W79+Exposed!W79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="X79" s="1" t="n">
+        <f aca="true" t="array" ref="X79:X79">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X79+Exposed!X79)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="n">
+        <v>44421</v>
+      </c>
+      <c r="B80" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="C80" s="1" t="n">
+        <f aca="true" t="array" ref="C80:C80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C80+Exposed!C80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>15</v>
+      </c>
+      <c r="D80" s="1" t="n">
+        <f aca="true" t="array" ref="D80:D80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D80+Exposed!D80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>6</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <f aca="true" t="array" ref="E80:E80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E80+Exposed!E80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>10</v>
+      </c>
+      <c r="F80" s="1" t="n">
+        <f aca="true" t="array" ref="F80:F80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F80+Exposed!F80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>6</v>
+      </c>
+      <c r="G80" s="1" t="n">
+        <f aca="true" t="array" ref="G80:G80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G80+Exposed!G80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>6</v>
+      </c>
+      <c r="H80" s="1" t="n">
+        <f aca="true" t="array" ref="H80:H80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H80+Exposed!H80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>4</v>
+      </c>
+      <c r="I80" s="1" t="n">
+        <f aca="true" t="array" ref="I80:I80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I80+Exposed!I80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>14</v>
+      </c>
+      <c r="J80" s="1" t="n">
+        <f aca="true" t="array" ref="J80:J80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J80+Exposed!J80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>22</v>
+      </c>
+      <c r="K80" s="1" t="n">
+        <f aca="true" t="array" ref="K80:K80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K80+Exposed!K80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>22</v>
+      </c>
+      <c r="L80" s="1" t="n">
+        <f aca="true" t="array" ref="L80:L80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L80+Exposed!L80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>17</v>
+      </c>
+      <c r="M80" s="1" t="n">
+        <f aca="true" t="array" ref="M80:M80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M80+Exposed!M80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>5</v>
+      </c>
+      <c r="N80" s="1" t="n">
+        <f aca="true" t="array" ref="N80:N80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N80+Exposed!N80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>9</v>
+      </c>
+      <c r="O80" s="1" t="n">
+        <f aca="true" t="array" ref="O80:O80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O80+Exposed!O80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>15</v>
+      </c>
+      <c r="P80" s="1" t="n">
+        <f aca="true" t="array" ref="P80:P80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P80+Exposed!P80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>2</v>
+      </c>
+      <c r="Q80" s="1" t="n">
+        <f aca="true" t="array" ref="Q80:Q80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q80+Exposed!Q80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>3</v>
+      </c>
+      <c r="R80" s="1" t="n">
+        <f aca="true" t="array" ref="R80:R80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R80+Exposed!R80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>9</v>
+      </c>
+      <c r="S80" s="1" t="n">
+        <f aca="true" t="array" ref="S80:S80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S80+Exposed!S80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="T80" s="1" t="n">
+        <f aca="true" t="array" ref="T80:T80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T80+Exposed!T80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>3</v>
+      </c>
+      <c r="U80" s="1" t="n">
+        <f aca="true" t="array" ref="U80:U80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U80+Exposed!U80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>2</v>
+      </c>
+      <c r="V80" s="1" t="n">
+        <f aca="true" t="array" ref="V80:V80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V80+Exposed!V80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>17</v>
+      </c>
+      <c r="W80" s="1" t="n">
+        <f aca="true" t="array" ref="W80:W80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W80+Exposed!W80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="X80" s="1" t="n">
+        <f aca="true" t="array" ref="X80:X80">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X80+Exposed!X80)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="n">
+        <v>44422</v>
+      </c>
+      <c r="B81" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <f aca="true" t="array" ref="C81:C81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C81+Exposed!C81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="D81" s="1" t="n">
+        <f aca="true" t="array" ref="D81:D81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D81+Exposed!D81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>25</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <f aca="true" t="array" ref="E81:E81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E81+Exposed!E81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="F81" s="1" t="n">
+        <f aca="true" t="array" ref="F81:F81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F81+Exposed!F81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>19</v>
+      </c>
+      <c r="G81" s="1" t="n">
+        <f aca="true" t="array" ref="G81:G81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G81+Exposed!G81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>8</v>
+      </c>
+      <c r="H81" s="1" t="n">
+        <f aca="true" t="array" ref="H81:H81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H81+Exposed!H81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>4</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <f aca="true" t="array" ref="I81:I81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I81+Exposed!I81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>16</v>
+      </c>
+      <c r="J81" s="1" t="n">
+        <f aca="true" t="array" ref="J81:J81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J81+Exposed!J81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>14</v>
+      </c>
+      <c r="K81" s="1" t="n">
+        <f aca="true" t="array" ref="K81:K81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K81+Exposed!K81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>22</v>
+      </c>
+      <c r="L81" s="1" t="n">
+        <f aca="true" t="array" ref="L81:L81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L81+Exposed!L81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>6</v>
+      </c>
+      <c r="M81" s="1" t="n">
+        <f aca="true" t="array" ref="M81:M81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M81+Exposed!M81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>7</v>
+      </c>
+      <c r="N81" s="1" t="n">
+        <f aca="true" t="array" ref="N81:N81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N81+Exposed!N81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>25</v>
+      </c>
+      <c r="O81" s="1" t="n">
+        <f aca="true" t="array" ref="O81:O81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O81+Exposed!O81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>17</v>
+      </c>
+      <c r="P81" s="1" t="n">
+        <f aca="true" t="array" ref="P81:P81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P81+Exposed!P81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>2</v>
+      </c>
+      <c r="Q81" s="1" t="n">
+        <f aca="true" t="array" ref="Q81:Q81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q81+Exposed!Q81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>15</v>
+      </c>
+      <c r="R81" s="1" t="n">
+        <f aca="true" t="array" ref="R81:R81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R81+Exposed!R81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>7</v>
+      </c>
+      <c r="S81" s="1" t="n">
+        <f aca="true" t="array" ref="S81:S81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S81+Exposed!S81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>8</v>
+      </c>
+      <c r="T81" s="1" t="n">
+        <f aca="true" t="array" ref="T81:T81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T81+Exposed!T81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>17</v>
+      </c>
+      <c r="U81" s="1" t="n">
+        <f aca="true" t="array" ref="U81:U81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U81+Exposed!U81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>6</v>
+      </c>
+      <c r="V81" s="1" t="n">
+        <f aca="true" t="array" ref="V81:V81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V81+Exposed!V81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>21</v>
+      </c>
+      <c r="W81" s="1" t="n">
+        <f aca="true" t="array" ref="W81:W81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W81+Exposed!W81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>10</v>
+      </c>
+      <c r="X81" s="1" t="n">
+        <f aca="true" t="array" ref="X81:X81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X81+Exposed!X81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>13</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>
@@ -26705,11 +28038,11 @@
   </sheetPr>
   <dimension ref="A1:X86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76:X77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.046875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
   </cols>
@@ -33681,7 +35014,7 @@
       </c>
       <c r="B73" s="9" t="n">
         <f aca="false">8926959 -SUM(Infectious!B73,Deaths!B73)</f>
-        <v>8923653</v>
+        <v>8923654</v>
       </c>
       <c r="C73" s="10" t="n">
         <f aca="false">139485-SUM(Infectious!C73,Deaths!C73)</f>
@@ -33713,7 +35046,7 @@
       </c>
       <c r="J73" s="9" t="n">
         <f aca="false">233223-SUM(Infectious!J73,Deaths!J73)</f>
-        <v>233090</v>
+        <v>233091</v>
       </c>
       <c r="K73" s="9" t="n">
         <f aca="false">208680-SUM(Infectious!K73,Deaths!K73)</f>
@@ -33778,63 +35111,63 @@
       </c>
       <c r="B74" s="9" t="n">
         <f aca="false">8926959 -SUM(Infectious!B74,Deaths!B74)</f>
-        <v>8923535</v>
+        <v>8923571</v>
       </c>
       <c r="C74" s="10" t="n">
         <f aca="false">139485-SUM(Infectious!C74,Deaths!C74)</f>
-        <v>139374</v>
+        <v>139375</v>
       </c>
       <c r="D74" s="9" t="n">
         <f aca="false">189258--SUM(Infectious!D74,Deaths!D74)</f>
-        <v>189417</v>
+        <v>189415</v>
       </c>
       <c r="E74" s="9" t="n">
         <f aca="false">173970-SUM(Infectious!E74,Deaths!E74)</f>
-        <v>173918</v>
+        <v>173919</v>
       </c>
       <c r="F74" s="9" t="n">
         <f aca="false">157920-SUM(Infectious!F74,Deaths!F74)</f>
-        <v>157840</v>
+        <v>157841</v>
       </c>
       <c r="G74" s="9" t="n">
         <f aca="false">232077-SUM(Infectious!G74,Deaths!G74)</f>
-        <v>231939</v>
+        <v>231940</v>
       </c>
       <c r="H74" s="9" t="n">
         <f aca="false">356380-SUM(Infectious!H74,Deaths!H74)</f>
-        <v>356310</v>
+        <v>356311</v>
       </c>
       <c r="I74" s="9" t="n">
         <f aca="false">422151-SUM(Infectious!I74,Deaths!I74)</f>
-        <v>421860</v>
+        <v>421864</v>
       </c>
       <c r="J74" s="9" t="n">
         <f aca="false">233223-SUM(Infectious!J74,Deaths!J74)</f>
-        <v>232909</v>
+        <v>232912</v>
       </c>
       <c r="K74" s="9" t="n">
         <f aca="false">208680-SUM(Infectious!K74,Deaths!K74)</f>
-        <v>208517</v>
+        <v>208518</v>
       </c>
       <c r="L74" s="9" t="n">
         <f aca="false">618365-SUM(Infectious!L74,Deaths!L74)</f>
-        <v>618063</v>
+        <v>618066</v>
       </c>
       <c r="M74" s="9" t="n">
         <f aca="false">702972-SUM(Infectious!M74,Deaths!M74)</f>
-        <v>702942</v>
+        <v>702943</v>
       </c>
       <c r="N74" s="9" t="n">
         <f aca="false">781417-SUM(Infectious!N74,Deaths!N74)</f>
-        <v>781283</v>
+        <v>781285</v>
       </c>
       <c r="O74" s="9" t="n">
         <f aca="false">495955-SUM(Infectious!O74,Deaths!O74)</f>
-        <v>495584</v>
+        <v>495588</v>
       </c>
       <c r="P74" s="9" t="n">
         <f aca="false">69326-SUM(Infectious!P74,Deaths!P74)</f>
-        <v>69295</v>
+        <v>69296</v>
       </c>
       <c r="Q74" s="9" t="n">
         <f aca="false">457275-SUM(Infectious!Q74,Deaths!Q74)</f>
@@ -33842,15 +35175,15 @@
       </c>
       <c r="R74" s="9" t="n">
         <f aca="false">671252-SUM(Infectious!R74,Deaths!R74)</f>
-        <v>671133</v>
+        <v>671134</v>
       </c>
       <c r="S74" s="9" t="n">
         <f aca="false">539227-SUM(Infectious!S74,Deaths!S74)</f>
-        <v>539059</v>
+        <v>539060</v>
       </c>
       <c r="T74" s="9" t="n">
         <f aca="false">205329-SUM(Infectious!T74,Deaths!T74)</f>
-        <v>205194</v>
+        <v>205196</v>
       </c>
       <c r="U74" s="9" t="n">
         <f aca="false">162148-SUM(Infectious!U74,Deaths!U74)</f>
@@ -33858,15 +35191,15 @@
       </c>
       <c r="V74" s="9" t="n">
         <f aca="false">470393-SUM(Infectious!V74,Deaths!V74)</f>
-        <v>470295</v>
+        <v>470296</v>
       </c>
       <c r="W74" s="9" t="n">
         <f aca="false">478786-SUM(Infectious!W74,Deaths!W74)</f>
-        <v>478596</v>
+        <v>478598</v>
       </c>
       <c r="X74" s="9" t="n">
         <f aca="false">1161370-SUM(Infectious!X74,Deaths!X74)</f>
-        <v>1160962</v>
+        <v>1160965</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33875,11 +35208,11 @@
       </c>
       <c r="B75" s="9" t="n">
         <f aca="false">8926959 -SUM(Infectious!B75,Deaths!B75)</f>
-        <v>8923603</v>
+        <v>8923590</v>
       </c>
       <c r="C75" s="10" t="n">
         <f aca="false">139485-SUM(Infectious!C75,Deaths!C75)</f>
-        <v>139307</v>
+        <v>139306</v>
       </c>
       <c r="D75" s="9" t="n">
         <f aca="false">189258--SUM(Infectious!D75,Deaths!D75)</f>
@@ -33891,7 +35224,7 @@
       </c>
       <c r="F75" s="9" t="n">
         <f aca="false">157920-SUM(Infectious!F75,Deaths!F75)</f>
-        <v>157688</v>
+        <v>157687</v>
       </c>
       <c r="G75" s="9" t="n">
         <f aca="false">232077-SUM(Infectious!G75,Deaths!G75)</f>
@@ -33903,11 +35236,11 @@
       </c>
       <c r="I75" s="9" t="n">
         <f aca="false">422151-SUM(Infectious!I75,Deaths!I75)</f>
-        <v>421529</v>
+        <v>421527</v>
       </c>
       <c r="J75" s="9" t="n">
         <f aca="false">233223-SUM(Infectious!J75,Deaths!J75)</f>
-        <v>233026</v>
+        <v>233025</v>
       </c>
       <c r="K75" s="9" t="n">
         <f aca="false">208680-SUM(Infectious!K75,Deaths!K75)</f>
@@ -33915,11 +35248,11 @@
       </c>
       <c r="L75" s="9" t="n">
         <f aca="false">618365-SUM(Infectious!L75,Deaths!L75)</f>
-        <v>618114</v>
+        <v>618113</v>
       </c>
       <c r="M75" s="9" t="n">
         <f aca="false">702972-SUM(Infectious!M75,Deaths!M75)</f>
-        <v>702941</v>
+        <v>702940</v>
       </c>
       <c r="N75" s="9" t="n">
         <f aca="false">781417-SUM(Infectious!N75,Deaths!N75)</f>
@@ -33927,7 +35260,7 @@
       </c>
       <c r="O75" s="9" t="n">
         <f aca="false">495955-SUM(Infectious!O75,Deaths!O75)</f>
-        <v>495785</v>
+        <v>495784</v>
       </c>
       <c r="P75" s="9" t="n">
         <f aca="false">69326-SUM(Infectious!P75,Deaths!P75)</f>
@@ -33939,11 +35272,11 @@
       </c>
       <c r="R75" s="9" t="n">
         <f aca="false">671252-SUM(Infectious!R75,Deaths!R75)</f>
-        <v>671152</v>
+        <v>671151</v>
       </c>
       <c r="S75" s="9" t="n">
         <f aca="false">539227-SUM(Infectious!S75,Deaths!S75)</f>
-        <v>539065</v>
+        <v>539064</v>
       </c>
       <c r="T75" s="9" t="n">
         <f aca="false">205329-SUM(Infectious!T75,Deaths!T75)</f>
@@ -33959,7 +35292,7 @@
       </c>
       <c r="W75" s="9" t="n">
         <f aca="false">478786-SUM(Infectious!W75,Deaths!W75)</f>
-        <v>478596</v>
+        <v>478595</v>
       </c>
       <c r="X75" s="9" t="n">
         <f aca="false">1161370-SUM(Infectious!X75,Deaths!X75)</f>
@@ -33972,27 +35305,27 @@
       </c>
       <c r="B76" s="9" t="n">
         <f aca="false">8926959 -SUM(Infectious!B76,Deaths!B76)</f>
-        <v>8923467</v>
+        <v>8923421</v>
       </c>
       <c r="C76" s="10" t="n">
         <f aca="false">139485-SUM(Infectious!C76,Deaths!C76)</f>
-        <v>139306</v>
+        <v>139304</v>
       </c>
       <c r="D76" s="9" t="n">
         <f aca="false">189258--SUM(Infectious!D76,Deaths!D76)</f>
-        <v>189330</v>
+        <v>189331</v>
       </c>
       <c r="E76" s="9" t="n">
         <f aca="false">173970-SUM(Infectious!E76,Deaths!E76)</f>
-        <v>173869</v>
+        <v>173867</v>
       </c>
       <c r="F76" s="9" t="n">
         <f aca="false">157920-SUM(Infectious!F76,Deaths!F76)</f>
-        <v>157605</v>
+        <v>157602</v>
       </c>
       <c r="G76" s="9" t="n">
         <f aca="false">232077-SUM(Infectious!G76,Deaths!G76)</f>
-        <v>231975</v>
+        <v>231973</v>
       </c>
       <c r="H76" s="9" t="n">
         <f aca="false">356380-SUM(Infectious!H76,Deaths!H76)</f>
@@ -34000,51 +35333,51 @@
       </c>
       <c r="I76" s="9" t="n">
         <f aca="false">422151-SUM(Infectious!I76,Deaths!I76)</f>
-        <v>421604</v>
+        <v>421596</v>
       </c>
       <c r="J76" s="9" t="n">
         <f aca="false">233223-SUM(Infectious!J76,Deaths!J76)</f>
-        <v>232892</v>
+        <v>232888</v>
       </c>
       <c r="K76" s="9" t="n">
         <f aca="false">208680-SUM(Infectious!K76,Deaths!K76)</f>
-        <v>208478</v>
+        <v>208475</v>
       </c>
       <c r="L76" s="9" t="n">
         <f aca="false">618365-SUM(Infectious!L76,Deaths!L76)</f>
-        <v>618176</v>
+        <v>618174</v>
       </c>
       <c r="M76" s="9" t="n">
         <f aca="false">702972-SUM(Infectious!M76,Deaths!M76)</f>
-        <v>702928</v>
+        <v>702927</v>
       </c>
       <c r="N76" s="9" t="n">
         <f aca="false">781417-SUM(Infectious!N76,Deaths!N76)</f>
-        <v>781357</v>
+        <v>781355</v>
       </c>
       <c r="O76" s="9" t="n">
         <f aca="false">495955-SUM(Infectious!O76,Deaths!O76)</f>
-        <v>495660</v>
+        <v>495657</v>
       </c>
       <c r="P76" s="9" t="n">
         <f aca="false">69326-SUM(Infectious!P76,Deaths!P76)</f>
-        <v>69253</v>
+        <v>69252</v>
       </c>
       <c r="Q76" s="9" t="n">
         <f aca="false">457275-SUM(Infectious!Q76,Deaths!Q76)</f>
-        <v>457126</v>
+        <v>457124</v>
       </c>
       <c r="R76" s="9" t="n">
         <f aca="false">671252-SUM(Infectious!R76,Deaths!R76)</f>
-        <v>671086</v>
+        <v>671084</v>
       </c>
       <c r="S76" s="9" t="n">
         <f aca="false">539227-SUM(Infectious!S76,Deaths!S76)</f>
-        <v>539075</v>
+        <v>539073</v>
       </c>
       <c r="T76" s="9" t="n">
         <f aca="false">205329-SUM(Infectious!T76,Deaths!T76)</f>
-        <v>205224</v>
+        <v>205223</v>
       </c>
       <c r="U76" s="9" t="n">
         <f aca="false">162148-SUM(Infectious!U76,Deaths!U76)</f>
@@ -34052,15 +35385,15 @@
       </c>
       <c r="V76" s="9" t="n">
         <f aca="false">470393-SUM(Infectious!V76,Deaths!V76)</f>
-        <v>470212</v>
+        <v>470210</v>
       </c>
       <c r="W76" s="9" t="n">
         <f aca="false">478786-SUM(Infectious!W76,Deaths!W76)</f>
-        <v>478671</v>
+        <v>478670</v>
       </c>
       <c r="X76" s="9" t="n">
         <f aca="false">1161370-SUM(Infectious!X76,Deaths!X76)</f>
-        <v>1161292</v>
+        <v>1161291</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34069,108 +35402,484 @@
       </c>
       <c r="B77" s="9" t="n">
         <f aca="false">8926959 -SUM(Infectious!B77,Deaths!B77)</f>
-        <v>8923291</v>
+        <v>8923207</v>
       </c>
       <c r="C77" s="10" t="n">
         <f aca="false">139485-SUM(Infectious!C77,Deaths!C77)</f>
-        <v>139251</v>
+        <v>139246</v>
       </c>
       <c r="D77" s="9" t="n">
         <f aca="false">189258--SUM(Infectious!D77,Deaths!D77)</f>
-        <v>189456</v>
+        <v>189461</v>
       </c>
       <c r="E77" s="9" t="n">
         <f aca="false">173970-SUM(Infectious!E77,Deaths!E77)</f>
-        <v>173770</v>
+        <v>173765</v>
       </c>
       <c r="F77" s="9" t="n">
         <f aca="false">157920-SUM(Infectious!F77,Deaths!F77)</f>
-        <v>157599</v>
+        <v>157592</v>
       </c>
       <c r="G77" s="9" t="n">
         <f aca="false">232077-SUM(Infectious!G77,Deaths!G77)</f>
-        <v>232027</v>
+        <v>232025</v>
       </c>
       <c r="H77" s="9" t="n">
         <f aca="false">356380-SUM(Infectious!H77,Deaths!H77)</f>
-        <v>356358</v>
+        <v>356357</v>
       </c>
       <c r="I77" s="9" t="n">
         <f aca="false">422151-SUM(Infectious!I77,Deaths!I77)</f>
-        <v>422044</v>
+        <v>422041</v>
       </c>
       <c r="J77" s="9" t="n">
         <f aca="false">233223-SUM(Infectious!J77,Deaths!J77)</f>
-        <v>233200</v>
+        <v>233199</v>
       </c>
       <c r="K77" s="9" t="n">
         <f aca="false">208680-SUM(Infectious!K77,Deaths!K77)</f>
-        <v>208434</v>
+        <v>208429</v>
       </c>
       <c r="L77" s="9" t="n">
         <f aca="false">618365-SUM(Infectious!L77,Deaths!L77)</f>
-        <v>617976</v>
+        <v>617967</v>
       </c>
       <c r="M77" s="9" t="n">
         <f aca="false">702972-SUM(Infectious!M77,Deaths!M77)</f>
-        <v>702935</v>
+        <v>702933</v>
       </c>
       <c r="N77" s="9" t="n">
         <f aca="false">781417-SUM(Infectious!N77,Deaths!N77)</f>
-        <v>781108</v>
+        <v>781101</v>
       </c>
       <c r="O77" s="9" t="n">
         <f aca="false">495955-SUM(Infectious!O77,Deaths!O77)</f>
-        <v>495641</v>
+        <v>495634</v>
       </c>
       <c r="P77" s="9" t="n">
         <f aca="false">69326-SUM(Infectious!P77,Deaths!P77)</f>
-        <v>69294</v>
+        <v>69293</v>
       </c>
       <c r="Q77" s="9" t="n">
         <f aca="false">457275-SUM(Infectious!Q77,Deaths!Q77)</f>
-        <v>457143</v>
+        <v>457139</v>
       </c>
       <c r="R77" s="9" t="n">
         <f aca="false">671252-SUM(Infectious!R77,Deaths!R77)</f>
-        <v>671064</v>
+        <v>671060</v>
       </c>
       <c r="S77" s="9" t="n">
         <f aca="false">539227-SUM(Infectious!S77,Deaths!S77)</f>
-        <v>539036</v>
+        <v>539033</v>
       </c>
       <c r="T77" s="9" t="n">
         <f aca="false">205329-SUM(Infectious!T77,Deaths!T77)</f>
-        <v>205267</v>
+        <v>205266</v>
       </c>
       <c r="U77" s="9" t="n">
         <f aca="false">162148-SUM(Infectious!U77,Deaths!U77)</f>
-        <v>162042</v>
+        <v>162040</v>
       </c>
       <c r="V77" s="9" t="n">
         <f aca="false">470393-SUM(Infectious!V77,Deaths!V77)</f>
-        <v>470188</v>
+        <v>470184</v>
       </c>
       <c r="W77" s="9" t="n">
         <f aca="false">478786-SUM(Infectious!W77,Deaths!W77)</f>
-        <v>478651</v>
+        <v>478648</v>
       </c>
       <c r="X77" s="9" t="n">
         <f aca="false">1161370-SUM(Infectious!X77,Deaths!X77)</f>
-        <v>1161204</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="80" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3"/>
+        <v>1161200</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="n">
+        <v>44419</v>
+      </c>
+      <c r="B78" s="9" t="n">
+        <f aca="false">8926959 -SUM(Infectious!B78,Deaths!B78)</f>
+        <v>8924320</v>
+      </c>
+      <c r="C78" s="10" t="n">
+        <f aca="false">139485-SUM(Infectious!C78,Deaths!C78)</f>
+        <v>139451</v>
+      </c>
+      <c r="D78" s="9" t="n">
+        <f aca="false">189258--SUM(Infectious!D78,Deaths!D78)</f>
+        <v>189345</v>
+      </c>
+      <c r="E78" s="9" t="n">
+        <f aca="false">173970-SUM(Infectious!E78,Deaths!E78)</f>
+        <v>173809</v>
+      </c>
+      <c r="F78" s="9" t="n">
+        <f aca="false">157920-SUM(Infectious!F78,Deaths!F78)</f>
+        <v>157889</v>
+      </c>
+      <c r="G78" s="9" t="n">
+        <f aca="false">232077-SUM(Infectious!G78,Deaths!G78)</f>
+        <v>232035</v>
+      </c>
+      <c r="H78" s="9" t="n">
+        <f aca="false">356380-SUM(Infectious!H78,Deaths!H78)</f>
+        <v>356319</v>
+      </c>
+      <c r="I78" s="9" t="n">
+        <f aca="false">422151-SUM(Infectious!I78,Deaths!I78)</f>
+        <v>422049</v>
+      </c>
+      <c r="J78" s="9" t="n">
+        <f aca="false">233223-SUM(Infectious!J78,Deaths!J78)</f>
+        <v>232995</v>
+      </c>
+      <c r="K78" s="9" t="n">
+        <f aca="false">208680-SUM(Infectious!K78,Deaths!K78)</f>
+        <v>208463</v>
+      </c>
+      <c r="L78" s="9" t="n">
+        <f aca="false">618365-SUM(Infectious!L78,Deaths!L78)</f>
+        <v>618061</v>
+      </c>
+      <c r="M78" s="9" t="n">
+        <f aca="false">702972-SUM(Infectious!M78,Deaths!M78)</f>
+        <v>702945</v>
+      </c>
+      <c r="N78" s="9" t="n">
+        <f aca="false">781417-SUM(Infectious!N78,Deaths!N78)</f>
+        <v>781349</v>
+      </c>
+      <c r="O78" s="9" t="n">
+        <f aca="false">495955-SUM(Infectious!O78,Deaths!O78)</f>
+        <v>495668</v>
+      </c>
+      <c r="P78" s="9" t="n">
+        <f aca="false">69326-SUM(Infectious!P78,Deaths!P78)</f>
+        <v>69305</v>
+      </c>
+      <c r="Q78" s="9" t="n">
+        <f aca="false">457275-SUM(Infectious!Q78,Deaths!Q78)</f>
+        <v>457074</v>
+      </c>
+      <c r="R78" s="9" t="n">
+        <f aca="false">671252-SUM(Infectious!R78,Deaths!R78)</f>
+        <v>671122</v>
+      </c>
+      <c r="S78" s="9" t="n">
+        <f aca="false">539227-SUM(Infectious!S78,Deaths!S78)</f>
+        <v>539098</v>
+      </c>
+      <c r="T78" s="9" t="n">
+        <f aca="false">205329-SUM(Infectious!T78,Deaths!T78)</f>
+        <v>205283</v>
+      </c>
+      <c r="U78" s="9" t="n">
+        <f aca="false">162148-SUM(Infectious!U78,Deaths!U78)</f>
+        <v>162144</v>
+      </c>
+      <c r="V78" s="9" t="n">
+        <f aca="false">470393-SUM(Infectious!V78,Deaths!V78)</f>
+        <v>470285</v>
+      </c>
+      <c r="W78" s="9" t="n">
+        <f aca="false">478786-SUM(Infectious!W78,Deaths!W78)</f>
+        <v>478643</v>
+      </c>
+      <c r="X78" s="9" t="n">
+        <f aca="false">1161370-SUM(Infectious!X78,Deaths!X78)</f>
+        <v>1161161</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="n">
+        <v>44420</v>
+      </c>
+      <c r="B79" s="9" t="n">
+        <f aca="false">8926959 -SUM(Infectious!B79,Deaths!B79)</f>
+        <v>8924314</v>
+      </c>
+      <c r="C79" s="10" t="n">
+        <f aca="false">139485-SUM(Infectious!C79,Deaths!C79)</f>
+        <v>139353</v>
+      </c>
+      <c r="D79" s="9" t="n">
+        <f aca="false">189258--SUM(Infectious!D79,Deaths!D79)</f>
+        <v>189353</v>
+      </c>
+      <c r="E79" s="9" t="n">
+        <f aca="false">173970-SUM(Infectious!E79,Deaths!E79)</f>
+        <v>173794</v>
+      </c>
+      <c r="F79" s="9" t="n">
+        <f aca="false">157920-SUM(Infectious!F79,Deaths!F79)</f>
+        <v>157811</v>
+      </c>
+      <c r="G79" s="9" t="n">
+        <f aca="false">232077-SUM(Infectious!G79,Deaths!G79)</f>
+        <v>232033</v>
+      </c>
+      <c r="H79" s="9" t="n">
+        <f aca="false">356380-SUM(Infectious!H79,Deaths!H79)</f>
+        <v>356352</v>
+      </c>
+      <c r="I79" s="9" t="n">
+        <f aca="false">422151-SUM(Infectious!I79,Deaths!I79)</f>
+        <v>422009</v>
+      </c>
+      <c r="J79" s="9" t="n">
+        <f aca="false">233223-SUM(Infectious!J79,Deaths!J79)</f>
+        <v>233207</v>
+      </c>
+      <c r="K79" s="9" t="n">
+        <f aca="false">208680-SUM(Infectious!K79,Deaths!K79)</f>
+        <v>208528</v>
+      </c>
+      <c r="L79" s="9" t="n">
+        <f aca="false">618365-SUM(Infectious!L79,Deaths!L79)</f>
+        <v>618128</v>
+      </c>
+      <c r="M79" s="9" t="n">
+        <f aca="false">702972-SUM(Infectious!M79,Deaths!M79)</f>
+        <v>702940</v>
+      </c>
+      <c r="N79" s="9" t="n">
+        <f aca="false">781417-SUM(Infectious!N79,Deaths!N79)</f>
+        <v>781307</v>
+      </c>
+      <c r="O79" s="9" t="n">
+        <f aca="false">495955-SUM(Infectious!O79,Deaths!O79)</f>
+        <v>495749</v>
+      </c>
+      <c r="P79" s="9" t="n">
+        <f aca="false">69326-SUM(Infectious!P79,Deaths!P79)</f>
+        <v>69324</v>
+      </c>
+      <c r="Q79" s="9" t="n">
+        <f aca="false">457275-SUM(Infectious!Q79,Deaths!Q79)</f>
+        <v>457043</v>
+      </c>
+      <c r="R79" s="9" t="n">
+        <f aca="false">671252-SUM(Infectious!R79,Deaths!R79)</f>
+        <v>671180</v>
+      </c>
+      <c r="S79" s="9" t="n">
+        <f aca="false">539227-SUM(Infectious!S79,Deaths!S79)</f>
+        <v>539065</v>
+      </c>
+      <c r="T79" s="9" t="n">
+        <f aca="false">205329-SUM(Infectious!T79,Deaths!T79)</f>
+        <v>205096</v>
+      </c>
+      <c r="U79" s="9" t="n">
+        <f aca="false">162148-SUM(Infectious!U79,Deaths!U79)</f>
+        <v>162033</v>
+      </c>
+      <c r="V79" s="9" t="n">
+        <f aca="false">470393-SUM(Infectious!V79,Deaths!V79)</f>
+        <v>470263</v>
+      </c>
+      <c r="W79" s="9" t="n">
+        <f aca="false">478786-SUM(Infectious!W79,Deaths!W79)</f>
+        <v>478629</v>
+      </c>
+      <c r="X79" s="9" t="n">
+        <f aca="false">1161370-SUM(Infectious!X79,Deaths!X79)</f>
+        <v>1161307</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="n">
+        <v>44421</v>
+      </c>
+      <c r="B80" s="9" t="n">
+        <f aca="false">8926959 -SUM(Infectious!B80,Deaths!B80)</f>
+        <v>8924458</v>
+      </c>
+      <c r="C80" s="10" t="n">
+        <f aca="false">139485-SUM(Infectious!C80,Deaths!C80)</f>
+        <v>139323</v>
+      </c>
+      <c r="D80" s="9" t="n">
+        <f aca="false">189258--SUM(Infectious!D80,Deaths!D80)</f>
+        <v>189334</v>
+      </c>
+      <c r="E80" s="9" t="n">
+        <f aca="false">173970-SUM(Infectious!E80,Deaths!E80)</f>
+        <v>173877</v>
+      </c>
+      <c r="F80" s="9" t="n">
+        <f aca="false">157920-SUM(Infectious!F80,Deaths!F80)</f>
+        <v>157839</v>
+      </c>
+      <c r="G80" s="9" t="n">
+        <f aca="false">232077-SUM(Infectious!G80,Deaths!G80)</f>
+        <v>232040</v>
+      </c>
+      <c r="H80" s="9" t="n">
+        <f aca="false">356380-SUM(Infectious!H80,Deaths!H80)</f>
+        <v>356342</v>
+      </c>
+      <c r="I80" s="9" t="n">
+        <f aca="false">422151-SUM(Infectious!I80,Deaths!I80)</f>
+        <v>422094</v>
+      </c>
+      <c r="J80" s="9" t="n">
+        <f aca="false">233223-SUM(Infectious!J80,Deaths!J80)</f>
+        <v>232890</v>
+      </c>
+      <c r="K80" s="9" t="n">
+        <f aca="false">208680-SUM(Infectious!K80,Deaths!K80)</f>
+        <v>208349</v>
+      </c>
+      <c r="L80" s="9" t="n">
+        <f aca="false">618365-SUM(Infectious!L80,Deaths!L80)</f>
+        <v>618105</v>
+      </c>
+      <c r="M80" s="9" t="n">
+        <f aca="false">702972-SUM(Infectious!M80,Deaths!M80)</f>
+        <v>702939</v>
+      </c>
+      <c r="N80" s="9" t="n">
+        <f aca="false">781417-SUM(Infectious!N80,Deaths!N80)</f>
+        <v>781376</v>
+      </c>
+      <c r="O80" s="9" t="n">
+        <f aca="false">495955-SUM(Infectious!O80,Deaths!O80)</f>
+        <v>495809</v>
+      </c>
+      <c r="P80" s="9" t="n">
+        <f aca="false">69326-SUM(Infectious!P80,Deaths!P80)</f>
+        <v>69312</v>
+      </c>
+      <c r="Q80" s="9" t="n">
+        <f aca="false">457275-SUM(Infectious!Q80,Deaths!Q80)</f>
+        <v>457237</v>
+      </c>
+      <c r="R80" s="9" t="n">
+        <f aca="false">671252-SUM(Infectious!R80,Deaths!R80)</f>
+        <v>671156</v>
+      </c>
+      <c r="S80" s="9" t="n">
+        <f aca="false">539227-SUM(Infectious!S80,Deaths!S80)</f>
+        <v>539070</v>
+      </c>
+      <c r="T80" s="9" t="n">
+        <f aca="false">205329-SUM(Infectious!T80,Deaths!T80)</f>
+        <v>205290</v>
+      </c>
+      <c r="U80" s="9" t="n">
+        <f aca="false">162148-SUM(Infectious!U80,Deaths!U80)</f>
+        <v>162136</v>
+      </c>
+      <c r="V80" s="9" t="n">
+        <f aca="false">470393-SUM(Infectious!V80,Deaths!V80)</f>
+        <v>470161</v>
+      </c>
+      <c r="W80" s="9" t="n">
+        <f aca="false">478786-SUM(Infectious!W80,Deaths!W80)</f>
+        <v>478723</v>
+      </c>
+      <c r="X80" s="9" t="n">
+        <f aca="false">1161370-SUM(Infectious!X80,Deaths!X80)</f>
+        <v>1161210</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="n">
+        <v>44422</v>
+      </c>
+      <c r="B81" s="9" t="n">
+        <f aca="false">8926959 -SUM(Infectious!B81,Deaths!B81)</f>
+        <v>8924132</v>
+      </c>
+      <c r="C81" s="10" t="n">
+        <f aca="false">139485-SUM(Infectious!C81,Deaths!C81)</f>
+        <v>139350</v>
+      </c>
+      <c r="D81" s="9" t="n">
+        <f aca="false">189258--SUM(Infectious!D81,Deaths!D81)</f>
+        <v>189454</v>
+      </c>
+      <c r="E81" s="9" t="n">
+        <f aca="false">173970-SUM(Infectious!E81,Deaths!E81)</f>
+        <v>173859</v>
+      </c>
+      <c r="F81" s="9" t="n">
+        <f aca="false">157920-SUM(Infectious!F81,Deaths!F81)</f>
+        <v>157656</v>
+      </c>
+      <c r="G81" s="9" t="n">
+        <f aca="false">232077-SUM(Infectious!G81,Deaths!G81)</f>
+        <v>232054</v>
+      </c>
+      <c r="H81" s="9" t="n">
+        <f aca="false">356380-SUM(Infectious!H81,Deaths!H81)</f>
+        <v>356350</v>
+      </c>
+      <c r="I81" s="9" t="n">
+        <f aca="false">422151-SUM(Infectious!I81,Deaths!I81)</f>
+        <v>422081</v>
+      </c>
+      <c r="J81" s="9" t="n">
+        <f aca="false">233223-SUM(Infectious!J81,Deaths!J81)</f>
+        <v>233056</v>
+      </c>
+      <c r="K81" s="9" t="n">
+        <f aca="false">208680-SUM(Infectious!K81,Deaths!K81)</f>
+        <v>208382</v>
+      </c>
+      <c r="L81" s="9" t="n">
+        <f aca="false">618365-SUM(Infectious!L81,Deaths!L81)</f>
+        <v>618298</v>
+      </c>
+      <c r="M81" s="9" t="n">
+        <f aca="false">702972-SUM(Infectious!M81,Deaths!M81)</f>
+        <v>702924</v>
+      </c>
+      <c r="N81" s="9" t="n">
+        <f aca="false">781417-SUM(Infectious!N81,Deaths!N81)</f>
+        <v>781236</v>
+      </c>
+      <c r="O81" s="9" t="n">
+        <f aca="false">495955-SUM(Infectious!O81,Deaths!O81)</f>
+        <v>495722</v>
+      </c>
+      <c r="P81" s="9" t="n">
+        <f aca="false">69326-SUM(Infectious!P81,Deaths!P81)</f>
+        <v>69301</v>
+      </c>
+      <c r="Q81" s="9" t="n">
+        <f aca="false">457275-SUM(Infectious!Q81,Deaths!Q81)</f>
+        <v>457180</v>
+      </c>
+      <c r="R81" s="9" t="n">
+        <f aca="false">671252-SUM(Infectious!R81,Deaths!R81)</f>
+        <v>671177</v>
+      </c>
+      <c r="S81" s="9" t="n">
+        <f aca="false">539227-SUM(Infectious!S81,Deaths!S81)</f>
+        <v>539152</v>
+      </c>
+      <c r="T81" s="9" t="n">
+        <f aca="false">205329-SUM(Infectious!T81,Deaths!T81)</f>
+        <v>205140</v>
+      </c>
+      <c r="U81" s="9" t="n">
+        <f aca="false">162148-SUM(Infectious!U81,Deaths!U81)</f>
+        <v>162074</v>
+      </c>
+      <c r="V81" s="9" t="n">
+        <f aca="false">470393-SUM(Infectious!V81,Deaths!V81)</f>
+        <v>470105</v>
+      </c>
+      <c r="W81" s="9" t="n">
+        <f aca="false">478786-SUM(Infectious!W81,Deaths!W81)</f>
+        <v>478748</v>
+      </c>
+      <c r="X81" s="9" t="n">
+        <f aca="false">1161370-SUM(Infectious!X81,Deaths!X81)</f>
+        <v>1161226</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>

</xml_diff>

<commit_message>
fix days in csv, new data 08.14
</commit_message>
<xml_diff>
--- a/COVID-19/HCM/SEIRD_data_12_7_2021.xlsx
+++ b/COVID-19/HCM/SEIRD_data_12_7_2021.xlsx
@@ -251,8 +251,8 @@
   </sheetPr>
   <dimension ref="A1:X83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6202,8 +6202,80 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3"/>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="n">
+        <v>44422</v>
+      </c>
+      <c r="B81" s="5" t="n">
+        <f aca="false">SUM(C81:X81)</f>
+        <v>1633</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="D81" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="F81" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="G81" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="H81" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="J81" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="K81" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="L81" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="M81" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="N81" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="O81" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="P81" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q81" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="R81" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="S81" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="T81" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="U81" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V81" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="W81" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="X81" s="1" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>
@@ -6229,8 +6301,8 @@
   </sheetPr>
   <dimension ref="A1:Z83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12226,8 +12298,80 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3"/>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="n">
+        <v>44422</v>
+      </c>
+      <c r="B81" s="1" t="n">
+        <f aca="false">SUM(C81:X81)</f>
+        <v>2542</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="D81" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F81" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="G81" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H81" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="J81" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="K81" s="1" t="n">
+        <v>276</v>
+      </c>
+      <c r="L81" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="M81" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="N81" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="O81" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="P81" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q81" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="R81" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="S81" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="T81" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="U81" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="V81" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="W81" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="X81" s="1" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>
@@ -12251,13 +12395,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y80"/>
+  <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="9.78"/>
@@ -19995,6 +20139,103 @@
         <v>121</v>
       </c>
     </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="7" t="n">
+        <v>44422</v>
+      </c>
+      <c r="B81" s="5" t="n">
+        <v>3417</v>
+      </c>
+      <c r="C81" s="8" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C81+Exposed!C81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>135</v>
+      </c>
+      <c r="D81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D81+Exposed!D81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>303</v>
+      </c>
+      <c r="E81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E81+Exposed!E81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>128</v>
+      </c>
+      <c r="F81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F81+Exposed!F81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>228</v>
+      </c>
+      <c r="G81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G81+Exposed!G81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>90</v>
+      </c>
+      <c r="H81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H81+Exposed!H81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>52</v>
+      </c>
+      <c r="I81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I81+Exposed!I81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>190</v>
+      </c>
+      <c r="J81" s="5" t="n">
+        <f aca="true">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J81+Exposed!J81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>162</v>
+      </c>
+      <c r="K81" s="5" t="n">
+        <f aca="true" t="array" ref="K81:K81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K81+Exposed!K81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>269</v>
+      </c>
+      <c r="L81" s="5" t="n">
+        <f aca="true" t="array" ref="L81:L81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L81+Exposed!L81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>66</v>
+      </c>
+      <c r="M81" s="5" t="n">
+        <f aca="true" t="array" ref="M81:M81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M81+Exposed!M81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>88</v>
+      </c>
+      <c r="N81" s="5" t="n">
+        <f aca="true" t="array" ref="N81:N81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N81+Exposed!N81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>305</v>
+      </c>
+      <c r="O81" s="5" t="n">
+        <f aca="true" t="array" ref="O81:O81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O81+Exposed!O81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>209</v>
+      </c>
+      <c r="P81" s="5" t="n">
+        <f aca="true" t="array" ref="P81:P81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P81+Exposed!P81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>29</v>
+      </c>
+      <c r="Q81" s="5" t="n">
+        <f aca="true" t="array" ref="Q81:Q81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q81+Exposed!Q81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>179</v>
+      </c>
+      <c r="R81" s="5" t="n">
+        <f aca="true" t="array" ref="R81:R81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R81+Exposed!R81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>83</v>
+      </c>
+      <c r="S81" s="5" t="n">
+        <f aca="true" t="array" ref="S81:S81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S81+Exposed!S81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>94</v>
+      </c>
+      <c r="T81" s="5" t="n">
+        <f aca="true" t="array" ref="T81:T81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T81+Exposed!T81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>210</v>
+      </c>
+      <c r="U81" s="5" t="n">
+        <f aca="true" t="array" ref="U81:U81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U81+Exposed!U81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>71</v>
+      </c>
+      <c r="V81" s="5" t="n">
+        <f aca="true" t="array" ref="V81:V81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V81+Exposed!V81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>257</v>
+      </c>
+      <c r="W81" s="5" t="n">
+        <f aca="true" t="array" ref="W81:W81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W81+Exposed!W81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>115</v>
+      </c>
+      <c r="X81" s="5" t="n">
+        <f aca="true" t="array" ref="X81:X81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X81+Exposed!X81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -20014,10 +20255,10 @@
   <dimension ref="A1:X82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B80" activeCellId="0" sqref="B80"/>
+      <selection pane="topLeft" activeCell="B81" activeCellId="0" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="1" width="11.57"/>
   </cols>
@@ -27680,8 +27921,101 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3"/>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="n">
+        <v>44422</v>
+      </c>
+      <c r="B81" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <f aca="true" t="array" ref="C81:C81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!C81+Exposed!C81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="D81" s="1" t="n">
+        <f aca="true" t="array" ref="D81:D81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!D81+Exposed!D81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>25</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <f aca="true" t="array" ref="E81:E81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!E81+Exposed!E81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>11</v>
+      </c>
+      <c r="F81" s="1" t="n">
+        <f aca="true" t="array" ref="F81:F81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!F81+Exposed!F81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>19</v>
+      </c>
+      <c r="G81" s="1" t="n">
+        <f aca="true" t="array" ref="G81:G81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!G81+Exposed!G81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>8</v>
+      </c>
+      <c r="H81" s="1" t="n">
+        <f aca="true" t="array" ref="H81:H81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!H81+Exposed!H81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>4</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <f aca="true" t="array" ref="I81:I81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!I81+Exposed!I81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>16</v>
+      </c>
+      <c r="J81" s="1" t="n">
+        <f aca="true" t="array" ref="J81:J81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!J81+Exposed!J81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>14</v>
+      </c>
+      <c r="K81" s="1" t="n">
+        <f aca="true" t="array" ref="K81:K81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!K81+Exposed!K81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>22</v>
+      </c>
+      <c r="L81" s="1" t="n">
+        <f aca="true" t="array" ref="L81:L81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!L81+Exposed!L81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>6</v>
+      </c>
+      <c r="M81" s="1" t="n">
+        <f aca="true" t="array" ref="M81:M81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!M81+Exposed!M81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>7</v>
+      </c>
+      <c r="N81" s="1" t="n">
+        <f aca="true" t="array" ref="N81:N81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!N81+Exposed!N81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>25</v>
+      </c>
+      <c r="O81" s="1" t="n">
+        <f aca="true" t="array" ref="O81:O81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!O81+Exposed!O81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>17</v>
+      </c>
+      <c r="P81" s="1" t="n">
+        <f aca="true" t="array" ref="P81:P81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!P81+Exposed!P81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>2</v>
+      </c>
+      <c r="Q81" s="1" t="n">
+        <f aca="true" t="array" ref="Q81:Q81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!Q81+Exposed!Q81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>15</v>
+      </c>
+      <c r="R81" s="1" t="n">
+        <f aca="true" t="array" ref="R81:R81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!R81+Exposed!R81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>7</v>
+      </c>
+      <c r="S81" s="1" t="n">
+        <f aca="true" t="array" ref="S81:S81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!S81+Exposed!S81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>8</v>
+      </c>
+      <c r="T81" s="1" t="n">
+        <f aca="true" t="array" ref="T81:T81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!T81+Exposed!T81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>17</v>
+      </c>
+      <c r="U81" s="1" t="n">
+        <f aca="true" t="array" ref="U81:U81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!U81+Exposed!U81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>6</v>
+      </c>
+      <c r="V81" s="1" t="n">
+        <f aca="true" t="array" ref="V81:V81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!V81+Exposed!V81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>21</v>
+      </c>
+      <c r="W81" s="1" t="n">
+        <f aca="true" t="array" ref="W81:W81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!W81+Exposed!W81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>10</v>
+      </c>
+      <c r="X81" s="1" t="n">
+        <f aca="true" t="array" ref="X81:X81">ROUND(INDIRECT("B"&amp;ROW())*(Infectious!X81+Exposed!X81)/(INDIRECT("Infectious.B"&amp;ROW())+INDIRECT("Exposed.B"&amp;ROW())),0)</f>
+        <v>13</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>
@@ -27705,10 +28039,10 @@
   <dimension ref="A1:X86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
   </cols>
@@ -35450,8 +35784,102 @@
         <v>1161210</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="n">
+        <v>44422</v>
+      </c>
+      <c r="B81" s="9" t="n">
+        <f aca="false">8926959 -SUM(Infectious!B81,Deaths!B81)</f>
+        <v>8924132</v>
+      </c>
+      <c r="C81" s="10" t="n">
+        <f aca="false">139485-SUM(Infectious!C81,Deaths!C81)</f>
+        <v>139350</v>
+      </c>
+      <c r="D81" s="9" t="n">
+        <f aca="false">189258--SUM(Infectious!D81,Deaths!D81)</f>
+        <v>189454</v>
+      </c>
+      <c r="E81" s="9" t="n">
+        <f aca="false">173970-SUM(Infectious!E81,Deaths!E81)</f>
+        <v>173859</v>
+      </c>
+      <c r="F81" s="9" t="n">
+        <f aca="false">157920-SUM(Infectious!F81,Deaths!F81)</f>
+        <v>157656</v>
+      </c>
+      <c r="G81" s="9" t="n">
+        <f aca="false">232077-SUM(Infectious!G81,Deaths!G81)</f>
+        <v>232054</v>
+      </c>
+      <c r="H81" s="9" t="n">
+        <f aca="false">356380-SUM(Infectious!H81,Deaths!H81)</f>
+        <v>356350</v>
+      </c>
+      <c r="I81" s="9" t="n">
+        <f aca="false">422151-SUM(Infectious!I81,Deaths!I81)</f>
+        <v>422081</v>
+      </c>
+      <c r="J81" s="9" t="n">
+        <f aca="false">233223-SUM(Infectious!J81,Deaths!J81)</f>
+        <v>233056</v>
+      </c>
+      <c r="K81" s="9" t="n">
+        <f aca="false">208680-SUM(Infectious!K81,Deaths!K81)</f>
+        <v>208382</v>
+      </c>
+      <c r="L81" s="9" t="n">
+        <f aca="false">618365-SUM(Infectious!L81,Deaths!L81)</f>
+        <v>618298</v>
+      </c>
+      <c r="M81" s="9" t="n">
+        <f aca="false">702972-SUM(Infectious!M81,Deaths!M81)</f>
+        <v>702924</v>
+      </c>
+      <c r="N81" s="9" t="n">
+        <f aca="false">781417-SUM(Infectious!N81,Deaths!N81)</f>
+        <v>781236</v>
+      </c>
+      <c r="O81" s="9" t="n">
+        <f aca="false">495955-SUM(Infectious!O81,Deaths!O81)</f>
+        <v>495722</v>
+      </c>
+      <c r="P81" s="9" t="n">
+        <f aca="false">69326-SUM(Infectious!P81,Deaths!P81)</f>
+        <v>69301</v>
+      </c>
+      <c r="Q81" s="9" t="n">
+        <f aca="false">457275-SUM(Infectious!Q81,Deaths!Q81)</f>
+        <v>457180</v>
+      </c>
+      <c r="R81" s="9" t="n">
+        <f aca="false">671252-SUM(Infectious!R81,Deaths!R81)</f>
+        <v>671177</v>
+      </c>
+      <c r="S81" s="9" t="n">
+        <f aca="false">539227-SUM(Infectious!S81,Deaths!S81)</f>
+        <v>539152</v>
+      </c>
+      <c r="T81" s="9" t="n">
+        <f aca="false">205329-SUM(Infectious!T81,Deaths!T81)</f>
+        <v>205140</v>
+      </c>
+      <c r="U81" s="9" t="n">
+        <f aca="false">162148-SUM(Infectious!U81,Deaths!U81)</f>
+        <v>162074</v>
+      </c>
+      <c r="V81" s="9" t="n">
+        <f aca="false">470393-SUM(Infectious!V81,Deaths!V81)</f>
+        <v>470105</v>
+      </c>
+      <c r="W81" s="9" t="n">
+        <f aca="false">478786-SUM(Infectious!W81,Deaths!W81)</f>
+        <v>478748</v>
+      </c>
+      <c r="X81" s="9" t="n">
+        <f aca="false">1161370-SUM(Infectious!X81,Deaths!X81)</f>
+        <v>1161226</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>

</xml_diff>